<commit_message>
trying the new system
</commit_message>
<xml_diff>
--- a/decision_data.xlsx
+++ b/decision_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2875FD5F-396C-4C3E-8F80-49B2073CDFDB}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{49299341-AA56-49CF-9BC5-48FFE20EBE45}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38160" yWindow="3735" windowWidth="21600" windowHeight="11385" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="decision_data" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="all_features-double_node" sheetId="14" r:id="rId6"/>
     <sheet name="data_no_higher_order" sheetId="15" r:id="rId7"/>
     <sheet name="increased_gain" sheetId="16" r:id="rId8"/>
+    <sheet name="schema_2" sheetId="17" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">decision_data!$A$1:$H$151</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1613" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="25">
   <si>
     <t>first_peak</t>
   </si>
@@ -100,6 +101,12 @@
   </si>
   <si>
     <t>skewness</t>
+  </si>
+  <si>
+    <t>second_peak</t>
+  </si>
+  <si>
+    <t>second_peak_2</t>
   </si>
 </sst>
 </file>
@@ -38554,7 +38561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC28BB55-25D6-4159-87A6-7B6071A1B196}">
   <dimension ref="A1:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
@@ -42518,4 +42525,3176 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE62A285-51F5-40B8-A2D0-C84873CEB519}">
+  <dimension ref="A1:M77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>-0.17961008691793301</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>-0.22444477383981501</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.30080979772323602</v>
+      </c>
+      <c r="J2">
+        <v>0.20629816933702999</v>
+      </c>
+      <c r="K2">
+        <v>0.37494805731889402</v>
+      </c>
+      <c r="L2">
+        <v>-0.23876825021275</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>-0.35861668636614102</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>-0.74762574291583805</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.35497164679200599</v>
+      </c>
+      <c r="J3">
+        <v>0.23993183156297701</v>
+      </c>
+      <c r="K3">
+        <v>0.43691047820428103</v>
+      </c>
+      <c r="L3">
+        <v>-0.31435683964461503</v>
+      </c>
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>-9.9722477300889997E-3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0.157315771439798</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0.30723520174042601</v>
+      </c>
+      <c r="J4">
+        <v>0.160853743786114</v>
+      </c>
+      <c r="K4">
+        <v>0.39148954402373398</v>
+      </c>
+      <c r="L4">
+        <v>0.21229444663330699</v>
+      </c>
+      <c r="M4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>-0.30049732235495302</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>-0.78481839453643398</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0.32624635266785301</v>
+      </c>
+      <c r="J5">
+        <v>0.218875879492166</v>
+      </c>
+      <c r="K5">
+        <v>0.406008093637376</v>
+      </c>
+      <c r="L5">
+        <v>-6.4843851910280003E-3</v>
+      </c>
+      <c r="M5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>-2.2481705954554999E-2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0.15736982006175801</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0.31191201982879002</v>
+      </c>
+      <c r="J6">
+        <v>0.23550246115041101</v>
+      </c>
+      <c r="K6">
+        <v>0.381249187886745</v>
+      </c>
+      <c r="L6">
+        <v>0.14835266560375401</v>
+      </c>
+      <c r="M6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>-0.23091984147660399</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>-0.75550781746829698</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0.32219887402674102</v>
+      </c>
+      <c r="J7">
+        <v>0.20011473460148699</v>
+      </c>
+      <c r="K7">
+        <v>0.38645813965949599</v>
+      </c>
+      <c r="L7">
+        <v>8.7651024879931996E-2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.401927196059787</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0.14962303804549601</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0.31094292652739502</v>
+      </c>
+      <c r="J8">
+        <v>0.173840302010454</v>
+      </c>
+      <c r="K8">
+        <v>0.37189673746081298</v>
+      </c>
+      <c r="L8">
+        <v>0.176105489567394</v>
+      </c>
+      <c r="M8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>-0.19543133656881601</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>-0.23482893444206401</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0.30791479122285897</v>
+      </c>
+      <c r="J9">
+        <v>0.16181458378576799</v>
+      </c>
+      <c r="K9">
+        <v>0.37623083666366702</v>
+      </c>
+      <c r="L9">
+        <v>0.10254563247543</v>
+      </c>
+      <c r="M9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>-0.30441172624907398</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0.22127413462884399</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0.30066803501024902</v>
+      </c>
+      <c r="J10">
+        <v>0.16090118395473399</v>
+      </c>
+      <c r="K10">
+        <v>0.37332139487256999</v>
+      </c>
+      <c r="L10">
+        <v>0.176220414851923</v>
+      </c>
+      <c r="M10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>-0.251789649096548</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>-0.68573215357512396</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0.30354513138497502</v>
+      </c>
+      <c r="J11">
+        <v>0.13381508982750401</v>
+      </c>
+      <c r="K11">
+        <v>0.37113216356826101</v>
+      </c>
+      <c r="L11">
+        <v>0.14868918021226399</v>
+      </c>
+      <c r="M11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0.39766098941782801</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0.118778017057615</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0.29692758351569298</v>
+      </c>
+      <c r="J12">
+        <v>0.133891118241694</v>
+      </c>
+      <c r="K12">
+        <v>0.36559245663176798</v>
+      </c>
+      <c r="L12">
+        <v>0.18946825831335501</v>
+      </c>
+      <c r="M12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>-0.233180526094657</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>-0.77561175607176303</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0.300642028806057</v>
+      </c>
+      <c r="J13">
+        <v>0.12955233721916501</v>
+      </c>
+      <c r="K13">
+        <v>0.37245901819834498</v>
+      </c>
+      <c r="L13">
+        <v>0.137591757963099</v>
+      </c>
+      <c r="M13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>-4.5938647990929997E-3</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0.133431620803516</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0.29812168224459701</v>
+      </c>
+      <c r="J14">
+        <v>0.116371596619122</v>
+      </c>
+      <c r="K14">
+        <v>0.37061752871736697</v>
+      </c>
+      <c r="L14">
+        <v>0.16601054616959801</v>
+      </c>
+      <c r="M14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>-0.218004449415866</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>-0.66884651221967495</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0.29557494412627699</v>
+      </c>
+      <c r="J15">
+        <v>0.10986020770343501</v>
+      </c>
+      <c r="K15">
+        <v>0.36872634321523001</v>
+      </c>
+      <c r="L15">
+        <v>0.130344919985003</v>
+      </c>
+      <c r="M15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1.1026967129625E-2</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0.13289585826366401</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0.28703701889827998</v>
+      </c>
+      <c r="J16">
+        <v>9.9521366108945006E-2</v>
+      </c>
+      <c r="K16">
+        <v>0.35626655546140701</v>
+      </c>
+      <c r="L16">
+        <v>0.16451383006376399</v>
+      </c>
+      <c r="M16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>-0.29137858995280902</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>-0.72505776603035299</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0.278455759329435</v>
+      </c>
+      <c r="J17">
+        <v>9.6697949017982995E-2</v>
+      </c>
+      <c r="K17">
+        <v>0.34922652104979302</v>
+      </c>
+      <c r="L17">
+        <v>0.131504898713554</v>
+      </c>
+      <c r="M17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0.38547382999882301</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0.101077796575131</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0.27767390944208298</v>
+      </c>
+      <c r="J18">
+        <v>9.7151158850333999E-2</v>
+      </c>
+      <c r="K18">
+        <v>0.34475223501444902</v>
+      </c>
+      <c r="L18">
+        <v>0.15643645488052399</v>
+      </c>
+      <c r="M18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>-0.24185836139733699</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>-0.85715442516332396</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0.28337926257683399</v>
+      </c>
+      <c r="J19">
+        <v>0.113998534244937</v>
+      </c>
+      <c r="K19">
+        <v>0.35394855692448401</v>
+      </c>
+      <c r="L19">
+        <v>0.119502963301895</v>
+      </c>
+      <c r="M19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>-0.32302530077242197</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>-0.71125635765697903</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0.32660649403275399</v>
+      </c>
+      <c r="J20">
+        <v>0.266772605442962</v>
+      </c>
+      <c r="K20">
+        <v>0.40740014271314401</v>
+      </c>
+      <c r="L20">
+        <v>-0.24456879780849899</v>
+      </c>
+      <c r="M20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0.313061013668818</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0.23237309621049099</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0.28374335572966097</v>
+      </c>
+      <c r="J21">
+        <v>0.32767475918883598</v>
+      </c>
+      <c r="K21">
+        <v>0.38316204041370999</v>
+      </c>
+      <c r="L21">
+        <v>0.100664910131698</v>
+      </c>
+      <c r="M21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>-0.17734098381944999</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>-0.71744051299182299</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0.27639072951014598</v>
+      </c>
+      <c r="J22">
+        <v>0.31802045155140901</v>
+      </c>
+      <c r="K22">
+        <v>0.38827733408787202</v>
+      </c>
+      <c r="L22">
+        <v>-2.5075794440729E-2</v>
+      </c>
+      <c r="M22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0.28621412456317902</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0.19573218393483499</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0.254714724095842</v>
+      </c>
+      <c r="J23">
+        <v>0.32817568927619001</v>
+      </c>
+      <c r="K23">
+        <v>0.35724353556362598</v>
+      </c>
+      <c r="L23">
+        <v>9.0990209811286998E-2</v>
+      </c>
+      <c r="M23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>-0.31796775199940303</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>-0.83749044915417103</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0.26503036225466797</v>
+      </c>
+      <c r="J24">
+        <v>0.318689938248997</v>
+      </c>
+      <c r="K24">
+        <v>0.37872263040383902</v>
+      </c>
+      <c r="L24">
+        <v>-2.6279497739145001E-2</v>
+      </c>
+      <c r="M24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>3.543024677083E-3</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0.17598592500263699</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0.25731871612829799</v>
+      </c>
+      <c r="J25">
+        <v>0.27521861741319298</v>
+      </c>
+      <c r="K25">
+        <v>0.36108981142837698</v>
+      </c>
+      <c r="L25">
+        <v>0.1024540203103</v>
+      </c>
+      <c r="M25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>-0.27265410961631498</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>-0.81647670360670599</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0.25718612214139702</v>
+      </c>
+      <c r="J26">
+        <v>0.26124017958662799</v>
+      </c>
+      <c r="K26">
+        <v>0.372633723770604</v>
+      </c>
+      <c r="L26">
+        <v>-2.4747258559656999E-2</v>
+      </c>
+      <c r="M26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>2.6755165391659998E-3</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0.198255836396074</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0.25685932490847102</v>
+      </c>
+      <c r="J27">
+        <v>0.27072925868730302</v>
+      </c>
+      <c r="K27">
+        <v>0.36677938028909102</v>
+      </c>
+      <c r="L27">
+        <v>4.1984573255447001E-2</v>
+      </c>
+      <c r="M27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>-0.221989884887</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>-0.242943971616045</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0.25970053326575698</v>
+      </c>
+      <c r="J28">
+        <v>0.25681291799568201</v>
+      </c>
+      <c r="K28">
+        <v>0.37037051391239201</v>
+      </c>
+      <c r="L28">
+        <v>-7.1420333888979996E-3</v>
+      </c>
+      <c r="M28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0.165037699958069</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0.20744017186190999</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0.25599449791114298</v>
+      </c>
+      <c r="J29">
+        <v>0.27041832593276599</v>
+      </c>
+      <c r="K29">
+        <v>0.36362269262924801</v>
+      </c>
+      <c r="L29">
+        <v>4.1621347903005E-2</v>
+      </c>
+      <c r="M29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>-0.31382335361477598</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>-0.77633552070589595</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0.26025738082684302</v>
+      </c>
+      <c r="J30">
+        <v>0.253172690175476</v>
+      </c>
+      <c r="K30">
+        <v>0.364724694033222</v>
+      </c>
+      <c r="L30">
+        <v>1.2080226520055999E-2</v>
+      </c>
+      <c r="M30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0.37025524374177199</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0.13484492024964401</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0.25977243249235799</v>
+      </c>
+      <c r="J31">
+        <v>0.233253656645805</v>
+      </c>
+      <c r="K31">
+        <v>0.36234604984758101</v>
+      </c>
+      <c r="L31">
+        <v>6.9788292721130005E-2</v>
+      </c>
+      <c r="M31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>-0.24398930753074999</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>-0.24027575724334399</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0.26604144652307299</v>
+      </c>
+      <c r="J32">
+        <v>0.23851561382192699</v>
+      </c>
+      <c r="K32">
+        <v>0.36997821971770001</v>
+      </c>
+      <c r="L32">
+        <v>2.2931345300098001E-2</v>
+      </c>
+      <c r="M32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>0.40394214235110598</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0.158808092884029</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0.26673116844922801</v>
+      </c>
+      <c r="J33">
+        <v>0.22613902137356501</v>
+      </c>
+      <c r="K33">
+        <v>0.36648023416437497</v>
+      </c>
+      <c r="L33">
+        <v>7.1165117711326997E-2</v>
+      </c>
+      <c r="M33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>-0.219674248772359</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>-0.270534248025809</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0.27047637718623302</v>
+      </c>
+      <c r="J34">
+        <v>0.20345063433996999</v>
+      </c>
+      <c r="K34">
+        <v>0.37311726583850202</v>
+      </c>
+      <c r="L34">
+        <v>2.9562340691050001E-2</v>
+      </c>
+      <c r="M34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0.28135104973533298</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0.30302817106063801</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0.26811656710135001</v>
+      </c>
+      <c r="J35">
+        <v>0.20381750860696199</v>
+      </c>
+      <c r="K35">
+        <v>0.36920690652858301</v>
+      </c>
+      <c r="L35">
+        <v>7.1535336341002995E-2</v>
+      </c>
+      <c r="M35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>-0.37001418335202602</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>-0.80588194611541297</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0.270398624280346</v>
+      </c>
+      <c r="J36">
+        <v>0.198392579879789</v>
+      </c>
+      <c r="K36">
+        <v>0.37090395057104802</v>
+      </c>
+      <c r="L36">
+        <v>3.9197036053515003E-2</v>
+      </c>
+      <c r="M36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0.28782173153181301</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>0.326325796370391</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0.26613675899356298</v>
+      </c>
+      <c r="J37">
+        <v>0.196595521821601</v>
+      </c>
+      <c r="K37">
+        <v>0.36577794050771301</v>
+      </c>
+      <c r="L37">
+        <v>8.1450214144696997E-2</v>
+      </c>
+      <c r="M37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>-0.28014425958998501</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>-0.186686597485648</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0.35421119597752698</v>
+      </c>
+      <c r="J38">
+        <v>4.4766610015816E-2</v>
+      </c>
+      <c r="K38">
+        <v>0.445178763825747</v>
+      </c>
+      <c r="L38">
+        <v>-0.35560241550828398</v>
+      </c>
+      <c r="M38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0.42228742906646199</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0.20709902780618</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0.31725160692633497</v>
+      </c>
+      <c r="J39">
+        <v>2.9864417981795999E-2</v>
+      </c>
+      <c r="K39">
+        <v>0.39609167401811302</v>
+      </c>
+      <c r="L39">
+        <v>0.19387199204165301</v>
+      </c>
+      <c r="M39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>-0.19123219261982699</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>-0.19340485215384501</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0.311105109758475</v>
+      </c>
+      <c r="J40">
+        <v>0.14929667436243499</v>
+      </c>
+      <c r="K40">
+        <v>0.39185902416034302</v>
+      </c>
+      <c r="L40">
+        <v>2.2115685253674001E-2</v>
+      </c>
+      <c r="M40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0.12991042248430601</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>-0.94505784292223904</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>0.27826474705230703</v>
+      </c>
+      <c r="J41">
+        <v>0.18544463972640801</v>
+      </c>
+      <c r="K41">
+        <v>0.37551617259919601</v>
+      </c>
+      <c r="L41">
+        <v>0.228042526841747</v>
+      </c>
+      <c r="M41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>-0.19419257766782899</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>-0.28079611332545101</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0.277023231003244</v>
+      </c>
+      <c r="J42">
+        <v>0.145207368356226</v>
+      </c>
+      <c r="K42">
+        <v>0.390509160482643</v>
+      </c>
+      <c r="L42">
+        <v>2.7589047107895E-2</v>
+      </c>
+      <c r="M42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0.13490848996386401</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>0.31112142935356502</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0.26891310618777797</v>
+      </c>
+      <c r="J43">
+        <v>0.19794670751931701</v>
+      </c>
+      <c r="K43">
+        <v>0.38388099970239098</v>
+      </c>
+      <c r="L43">
+        <v>0.12815291520140201</v>
+      </c>
+      <c r="M43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>-0.18449870619332001</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>-0.75988596147770004</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0.258668502182621</v>
+      </c>
+      <c r="J44">
+        <v>0.183937925987915</v>
+      </c>
+      <c r="K44">
+        <v>0.37329699921184001</v>
+      </c>
+      <c r="L44">
+        <v>4.3971099375522002E-2</v>
+      </c>
+      <c r="M44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>0.362297806862312</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>-1.5472212760408099</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0.25591264358820098</v>
+      </c>
+      <c r="J45">
+        <v>0.18284394123210301</v>
+      </c>
+      <c r="K45">
+        <v>0.37535737873355102</v>
+      </c>
+      <c r="L45">
+        <v>0.13885020830835401</v>
+      </c>
+      <c r="M45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>-0.214285313840342</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>-0.76243147492395202</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0.25890861244788899</v>
+      </c>
+      <c r="J46">
+        <v>0.174235659728389</v>
+      </c>
+      <c r="K46">
+        <v>0.375971246446626</v>
+      </c>
+      <c r="L46">
+        <v>9.8316969859528994E-2</v>
+      </c>
+      <c r="M46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>-0.180349008566419</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>-0.77049753320190995</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0.25513486406846803</v>
+      </c>
+      <c r="J47">
+        <v>0.16569313985276801</v>
+      </c>
+      <c r="K47">
+        <v>0.37140119809871203</v>
+      </c>
+      <c r="L47">
+        <v>0.108387042426431</v>
+      </c>
+      <c r="M47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>0.31003417498951802</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>0.219775864815587</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0.25023268966373702</v>
+      </c>
+      <c r="J48">
+        <v>0.16358300493412101</v>
+      </c>
+      <c r="K48">
+        <v>0.36180599638938199</v>
+      </c>
+      <c r="L48">
+        <v>0.15232283801552801</v>
+      </c>
+      <c r="M48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>-0.37433216674394398</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>-0.95492233481238897</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0.26344884830099502</v>
+      </c>
+      <c r="J49">
+        <v>0.169129065081255</v>
+      </c>
+      <c r="K49">
+        <v>0.38042468144365099</v>
+      </c>
+      <c r="L49">
+        <v>5.6764036264467001E-2</v>
+      </c>
+      <c r="M49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>-2.7011057033119999E-3</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>0.14703864856452101</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>0.26204655977073399</v>
+      </c>
+      <c r="J50">
+        <v>0.153525893242133</v>
+      </c>
+      <c r="K50">
+        <v>0.37334030359231501</v>
+      </c>
+      <c r="L50">
+        <v>8.1983213829308996E-2</v>
+      </c>
+      <c r="M50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>-0.208984126771075</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>-0.87554947402950001</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0.267622497920527</v>
+      </c>
+      <c r="J51">
+        <v>0.147581901132258</v>
+      </c>
+      <c r="K51">
+        <v>0.38071959272912598</v>
+      </c>
+      <c r="L51">
+        <v>3.6810057359334E-2</v>
+      </c>
+      <c r="M51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0.354412200284002</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>0.224978742289622</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0.26564834018474598</v>
+      </c>
+      <c r="J52">
+        <v>0.14133904593070401</v>
+      </c>
+      <c r="K52">
+        <v>0.37655064805017902</v>
+      </c>
+      <c r="L52">
+        <v>8.8191276278658998E-2</v>
+      </c>
+      <c r="M52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>-0.23176181892981301</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>-0.82451104713145296</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0.26835354581718601</v>
+      </c>
+      <c r="J53">
+        <v>0.13005903381245801</v>
+      </c>
+      <c r="K53">
+        <v>0.37794523907127697</v>
+      </c>
+      <c r="L53">
+        <v>5.9482542254067003E-2</v>
+      </c>
+      <c r="M53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>7.3325810878669996E-3</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>0.246821069055632</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0.26859076242579899</v>
+      </c>
+      <c r="J54">
+        <v>0.11909406599783399</v>
+      </c>
+      <c r="K54">
+        <v>0.377854095938639</v>
+      </c>
+      <c r="L54">
+        <v>8.1952726189424993E-2</v>
+      </c>
+      <c r="M54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>-0.249691451397072</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>-0.253767878491367</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0.45025839710764098</v>
+      </c>
+      <c r="J55">
+        <v>0.290499754762363</v>
+      </c>
+      <c r="K55">
+        <v>0.60337639746206095</v>
+      </c>
+      <c r="L55">
+        <v>-0.27503656017775902</v>
+      </c>
+      <c r="M55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>-9.2471346860200005E-4</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>0.21976515512744901</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0.37895422412228003</v>
+      </c>
+      <c r="J56">
+        <v>0.19371287437800599</v>
+      </c>
+      <c r="K56">
+        <v>0.52652982546375005</v>
+      </c>
+      <c r="L56">
+        <v>0.16500316214207</v>
+      </c>
+      <c r="M56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>-0.19042586432973599</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>-0.25720935341865397</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0.38226854987791697</v>
+      </c>
+      <c r="J57">
+        <v>0.19382104940849501</v>
+      </c>
+      <c r="K57">
+        <v>0.51962390139124903</v>
+      </c>
+      <c r="L57">
+        <v>5.1889544872777998E-2</v>
+      </c>
+      <c r="M57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>-7.4656273037180003E-3</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>-1.2715783350474999E-2</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>9.9441013090804997E-2</v>
+      </c>
+      <c r="J58">
+        <v>0.155293989829317</v>
+      </c>
+      <c r="K58">
+        <v>0.12884778341810799</v>
+      </c>
+      <c r="L58">
+        <v>0.28789362862538997</v>
+      </c>
+      <c r="M58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>-0.26011147093894799</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>-0.82300331443618602</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0.11373955963804699</v>
+      </c>
+      <c r="J59">
+        <v>0.14375223729282599</v>
+      </c>
+      <c r="K59">
+        <v>0.14904150781616299</v>
+      </c>
+      <c r="L59">
+        <v>6.1148883320508003E-2</v>
+      </c>
+      <c r="M59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>3.5128905576049998E-3</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>7.9547263855553996E-2</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0.12524431291945301</v>
+      </c>
+      <c r="J60">
+        <v>0.120233141941177</v>
+      </c>
+      <c r="K60">
+        <v>0.160438450228581</v>
+      </c>
+      <c r="L60">
+        <v>0.17031643888116599</v>
+      </c>
+      <c r="M60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>-0.230119975366854</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>-0.29993677242301597</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0.48364766023236599</v>
+      </c>
+      <c r="J61">
+        <v>0.23698745092892301</v>
+      </c>
+      <c r="K61">
+        <v>0.63093912169672794</v>
+      </c>
+      <c r="L61">
+        <v>-0.38822685064985901</v>
+      </c>
+      <c r="M61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>-8.7849669519799996E-4</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>0.21383921035150699</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0.36819616273674999</v>
+      </c>
+      <c r="J62">
+        <v>0.28300571858988099</v>
+      </c>
+      <c r="K62">
+        <v>0.49294691288783399</v>
+      </c>
+      <c r="L62">
+        <v>-5.6303776959872001E-2</v>
+      </c>
+      <c r="M62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>-0.18480559518807901</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>-0.27192107084678402</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0.35449271522515102</v>
+      </c>
+      <c r="J63">
+        <v>0.21871662326888999</v>
+      </c>
+      <c r="K63">
+        <v>0.48377471901569202</v>
+      </c>
+      <c r="L63">
+        <v>-0.13661519906015199</v>
+      </c>
+      <c r="M63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>-5.2391295947639997E-3</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>0.15694755637224</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0.33191740940702102</v>
+      </c>
+      <c r="J64">
+        <v>0.13743942203635701</v>
+      </c>
+      <c r="K64">
+        <v>0.428816842479817</v>
+      </c>
+      <c r="L64">
+        <v>1.6467556205887999E-2</v>
+      </c>
+      <c r="M64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>-0.23909420728869801</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>-0.238766089230915</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0.33243042010868101</v>
+      </c>
+      <c r="J65">
+        <v>0.121599693271347</v>
+      </c>
+      <c r="K65">
+        <v>0.42778531257173702</v>
+      </c>
+      <c r="L65">
+        <v>-3.2123081002950998E-2</v>
+      </c>
+      <c r="M65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>-1.6152664199044001E-2</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>0.16072360957579701</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0.31992833203300902</v>
+      </c>
+      <c r="J66">
+        <v>0.105029495648575</v>
+      </c>
+      <c r="K66">
+        <v>0.406905276729634</v>
+      </c>
+      <c r="L66">
+        <v>5.8982726123467E-2</v>
+      </c>
+      <c r="M66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>-0.29240072332749001</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0.23431987699307699</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0.31016865817645001</v>
+      </c>
+      <c r="J67">
+        <v>0.114617008469063</v>
+      </c>
+      <c r="K67">
+        <v>0.39841185574705101</v>
+      </c>
+      <c r="L67">
+        <v>2.0573520365719999E-3</v>
+      </c>
+      <c r="M67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>0</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>0.43473067686844502</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>6.3392340905295996E-2</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>0.305326674803795</v>
+      </c>
+      <c r="J68">
+        <v>6.6956602298675005E-2</v>
+      </c>
+      <c r="K68">
+        <v>0.38497162838295801</v>
+      </c>
+      <c r="L68">
+        <v>6.7492519000386997E-2</v>
+      </c>
+      <c r="M68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>-0.32523041964957899</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>-0.19790387832954101</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0.30532550942895498</v>
+      </c>
+      <c r="J69">
+        <v>7.1224930913854997E-2</v>
+      </c>
+      <c r="K69">
+        <v>0.38396296171858002</v>
+      </c>
+      <c r="L69">
+        <v>1.4335506631377001E-2</v>
+      </c>
+      <c r="M69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>8.6586184933039999E-3</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>0.109037645593087</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0.30205321440319</v>
+      </c>
+      <c r="J70">
+        <v>7.0048958913121004E-2</v>
+      </c>
+      <c r="K70">
+        <v>0.37696038762668399</v>
+      </c>
+      <c r="L70">
+        <v>6.9574953873796003E-2</v>
+      </c>
+      <c r="M70" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>-0.206989148604456</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>-0.29485253954148899</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0.30086916105929001</v>
+      </c>
+      <c r="J71">
+        <v>7.1885852609734999E-2</v>
+      </c>
+      <c r="K71">
+        <v>0.38236331732881601</v>
+      </c>
+      <c r="L71">
+        <v>2.9179639066661E-2</v>
+      </c>
+      <c r="M71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>-0.19735439713903299</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>0.23164399539137101</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>0.29523894395113198</v>
+      </c>
+      <c r="J72">
+        <v>9.2196740276461006E-2</v>
+      </c>
+      <c r="K72">
+        <v>0.373917222660823</v>
+      </c>
+      <c r="L72">
+        <v>4.8684593773887001E-2</v>
+      </c>
+      <c r="M72" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>-0.22217398820197501</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>-0.274535033568995</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0.28647895475967</v>
+      </c>
+      <c r="J73">
+        <v>9.0929649062522003E-2</v>
+      </c>
+      <c r="K73">
+        <v>0.36561094209198902</v>
+      </c>
+      <c r="L73">
+        <v>1.8118859078443999E-2</v>
+      </c>
+      <c r="M73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>0</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>0.24151181180342601</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>0.27713635452072399</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>0.27904809026010802</v>
+      </c>
+      <c r="J74">
+        <v>0.10914946453785</v>
+      </c>
+      <c r="K74">
+        <v>0.356639484666053</v>
+      </c>
+      <c r="L74">
+        <v>5.4975844728038001E-2</v>
+      </c>
+      <c r="M74" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>1</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>-0.22564130713966499</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>-0.81314440233484797</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0.277602096730865</v>
+      </c>
+      <c r="J75">
+        <v>0.118736906995344</v>
+      </c>
+      <c r="K75">
+        <v>0.35846727525962802</v>
+      </c>
+      <c r="L75">
+        <v>2.2435271010955E-2</v>
+      </c>
+      <c r="M75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>0</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>0.28246278808249098</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>0.27680412807958499</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>0.27419033400009102</v>
+      </c>
+      <c r="J76">
+        <v>0.124624022623448</v>
+      </c>
+      <c r="K76">
+        <v>0.35444581376419099</v>
+      </c>
+      <c r="L76">
+        <v>5.0460927444269998E-2</v>
+      </c>
+      <c r="M76" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>-0.20780444793959299</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>-0.79739662548118895</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0.27448720349278499</v>
+      </c>
+      <c r="J77">
+        <v>0.13018852579708301</v>
+      </c>
+      <c r="K77">
+        <v>0.35760795787956301</v>
+      </c>
+      <c r="L77">
+        <v>1.9709668592304001E-2</v>
+      </c>
+      <c r="M77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
there are merge issues
</commit_message>
<xml_diff>
--- a/decision_data.xlsx
+++ b/decision_data.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="30" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AC3431A2-E8AE-4FC4-991E-BF2D88A2C91D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="decision_data" sheetId="1" r:id="rId1"/>
@@ -6563,8 +6563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909D9306-7CC2-4811-A201-EA3B40165022}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46062,7 +46062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE62A285-51F5-40B8-A2D0-C84873CEB519}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I121"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
have new model. Created with data when close to the sensor
</commit_message>
<xml_diff>
--- a/decision_data.xlsx
+++ b/decision_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AC3431A2-E8AE-4FC4-991E-BF2D88A2C91D}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{6089C275-0D90-4686-A462-31C4075F452C}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="1140" windowWidth="19200" windowHeight="11385" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="decision_data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="27">
   <si>
     <t>first_peak</t>
   </si>
@@ -46060,10 +46060,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE62A285-51F5-40B8-A2D0-C84873CEB519}">
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I121"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46105,7 +46105,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>-0.13444201866398101</v>
+        <v>-0.134442019</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -46114,7 +46114,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>-0.15133518107074501</v>
+        <v>-0.15133518100000001</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -46134,7 +46134,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>6.0159469682047002E-2</v>
+        <v>6.015947E-2</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -46143,7 +46143,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>0.11171848257962801</v>
+        <v>0.11171848299999999</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -46163,7 +46163,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>-0.11870922764802599</v>
+        <v>-0.118709228</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -46172,7 +46172,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>-0.42912442290857</v>
+        <v>-0.42912442299999998</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -46192,7 +46192,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>2.2964292925891999E-2</v>
+        <v>2.2964293E-2</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -46201,7 +46201,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>6.9158161297062995E-2</v>
+        <v>6.9158160999999996E-2</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -46221,7 +46221,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>-0.171887125231866</v>
+        <v>-0.171887125</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -46230,7 +46230,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>-0.126629040927692</v>
+        <v>-0.126629041</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -46250,7 +46250,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>-0.144720663820917</v>
+        <v>-0.144720664</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -46259,7 +46259,7 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>0.30448439358781998</v>
+        <v>0.30448439399999999</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -46279,7 +46279,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>6.4896550725600993E-2</v>
+        <v>6.4896550999999997E-2</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -46288,7 +46288,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>-6.3777235698478998E-2</v>
+        <v>-6.3777236000000001E-2</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -46308,7 +46308,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>4.5391520343475003E-2</v>
+        <v>4.5391519999999998E-2</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -46317,7 +46317,7 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>0.122332643628892</v>
+        <v>0.122332644</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -46337,7 +46337,7 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0.51005194905755702</v>
+        <v>0.51005194899999995</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -46346,7 +46346,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>-8.5903486157062003E-2</v>
+        <v>-8.5903486000000001E-2</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -46366,7 +46366,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>1.3206086540862E-2</v>
+        <v>1.3206087E-2</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -46375,7 +46375,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>-0.144321962982394</v>
+        <v>-0.144321963</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -46395,7 +46395,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>8.1722622681685994E-2</v>
+        <v>8.1722622999999994E-2</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -46404,7 +46404,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>-6.2441730577661003E-2</v>
+        <v>-6.2441731E-2</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -46424,7 +46424,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>4.0091816517151997E-2</v>
+        <v>4.0091817000000002E-2</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -46433,7 +46433,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>0.19180810236540499</v>
+        <v>0.19180810200000001</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -46453,7 +46453,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>-0.10906168584768</v>
+        <v>-0.109061686</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -46462,7 +46462,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>-0.42009364036820002</v>
+        <v>-0.42009363999999999</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -46482,7 +46482,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>8.3259552498954004E-2</v>
+        <v>8.3259552000000001E-2</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -46491,7 +46491,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>-0.18497658617351001</v>
+        <v>-0.184976586</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -46511,7 +46511,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>-0.23133933401989201</v>
+        <v>-0.23133933400000001</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -46520,7 +46520,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>-0.165371163602549</v>
+        <v>-0.16537116399999999</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -46540,7 +46540,7 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>0.141550210389773</v>
+        <v>0.14155021000000001</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -46549,7 +46549,7 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>0.35804491458431797</v>
+        <v>0.35804491500000002</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -46569,7 +46569,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>-0.25500355151994197</v>
+        <v>-0.25500355200000002</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -46578,7 +46578,7 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>-0.158434707802768</v>
+        <v>-0.15843470800000001</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -46598,7 +46598,7 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>0.16400944992288899</v>
+        <v>0.16400945</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -46607,7 +46607,7 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>0.36157309686938799</v>
+        <v>0.36157309700000001</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -46627,7 +46627,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>-0.20935399242932701</v>
+        <v>-0.20935399199999999</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -46636,7 +46636,7 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <v>0.13435816617684601</v>
+        <v>0.134358166</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -46656,7 +46656,7 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>0.17206906406297801</v>
+        <v>0.17206906399999999</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -46665,7 +46665,7 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>0.15587547968787799</v>
+        <v>0.15587548000000001</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -46685,7 +46685,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>-0.16263812072032899</v>
+        <v>-0.162638121</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -46694,7 +46694,7 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>0.15801340880009301</v>
+        <v>0.15801340899999999</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -46714,7 +46714,7 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>0.15252763227504701</v>
+        <v>0.152527632</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -46723,7 +46723,7 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <v>-4.2487757242789997E-2</v>
+        <v>-4.2487757000000001E-2</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -46743,7 +46743,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>-0.117814171421394</v>
+        <v>-0.117814171</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -46752,7 +46752,7 @@
         <v>1</v>
       </c>
       <c r="F24">
-        <v>0.11275617177679501</v>
+        <v>0.112756172</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -46772,7 +46772,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>-1.8414931372395998E-2</v>
+        <v>-1.8414930999999999E-2</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -46781,7 +46781,7 @@
         <v>1</v>
       </c>
       <c r="F25">
-        <v>-3.3397464334143999E-2</v>
+        <v>-3.3397464000000002E-2</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -46801,7 +46801,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>0.12545094050556799</v>
+        <v>0.12545094100000001</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -46810,7 +46810,7 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>0.10940432564737999</v>
+        <v>0.109404326</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -46830,7 +46830,7 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>0.176714137535634</v>
+        <v>0.17671413799999999</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -46839,7 +46839,7 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>-0.14086243582480301</v>
+        <v>-0.14086243600000001</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -46859,7 +46859,7 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <v>2.2526596868187001E-2</v>
+        <v>2.2526596999999999E-2</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -46868,7 +46868,7 @@
         <v>1</v>
       </c>
       <c r="F28">
-        <v>0.209552118869581</v>
+        <v>0.20955211900000001</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -46888,7 +46888,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>-4.1960853757126E-2</v>
+        <v>-4.1960853999999999E-2</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -46897,7 +46897,7 @@
         <v>1</v>
       </c>
       <c r="F29">
-        <v>9.3415148633384001E-2</v>
+        <v>9.3415149000000003E-2</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -46917,7 +46917,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <v>-0.102635177218489</v>
+        <v>-0.10263517699999999</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -46926,7 +46926,7 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <v>0.135876398827637</v>
+        <v>0.13587639900000001</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -46946,7 +46946,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>-9.3576433148900005E-4</v>
+        <v>-9.3576399999999995E-4</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -46955,7 +46955,7 @@
         <v>1</v>
       </c>
       <c r="F31">
-        <v>-4.8119228193510999E-2</v>
+        <v>-4.8119228E-2</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -46975,7 +46975,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <v>-0.17148925560665201</v>
+        <v>-0.17148925600000001</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -46984,7 +46984,7 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <v>0.20413363419272401</v>
+        <v>0.20413363400000001</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -47004,7 +47004,7 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>0.135863144844344</v>
+        <v>0.13586314499999999</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -47013,7 +47013,7 @@
         <v>1</v>
       </c>
       <c r="F33">
-        <v>3.3882108072132003E-2</v>
+        <v>3.3882108000000001E-2</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -47033,7 +47033,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>-0.15223832082091901</v>
+        <v>-0.15223832100000001</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -47042,7 +47042,7 @@
         <v>1</v>
       </c>
       <c r="F34">
-        <v>-0.10770773321409</v>
+        <v>-0.107707733</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -47062,7 +47062,7 @@
         <v>1</v>
       </c>
       <c r="C35">
-        <v>0.15538632329948501</v>
+        <v>0.15538632299999999</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -47071,7 +47071,7 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <v>-3.2439998912852E-2</v>
+        <v>-3.2439998999999997E-2</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -47091,7 +47091,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>-0.11898951861384</v>
+        <v>-0.118989519</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -47100,7 +47100,7 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>-0.40923130184600798</v>
+        <v>-0.40923130200000002</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -47120,7 +47120,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>3.6338152191158997E-2</v>
+        <v>3.6338151999999999E-2</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -47129,7 +47129,7 @@
         <v>1</v>
       </c>
       <c r="F37">
-        <v>0.100849279713009</v>
+        <v>0.10084928</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -47149,7 +47149,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>-0.119135391597137</v>
+        <v>-0.11913539200000001</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -47158,7 +47158,7 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>-5.5394059569297001E-2</v>
+        <v>-5.5394060000000002E-2</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -47178,7 +47178,7 @@
         <v>1</v>
       </c>
       <c r="C39">
-        <v>0.17459927614739601</v>
+        <v>0.174599276</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -47187,7 +47187,7 @@
         <v>1</v>
       </c>
       <c r="F39">
-        <v>-6.5027584615896999E-2</v>
+        <v>-6.5027584999999999E-2</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -47207,7 +47207,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>-0.11376205798990099</v>
+        <v>-0.113762058</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -47216,7 +47216,7 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>-7.2061258519043006E-2</v>
+        <v>-7.2061259000000003E-2</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -47236,7 +47236,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>6.7207223935079996E-2</v>
+        <v>6.7207223999999996E-2</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -47245,7 +47245,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>-0.20000679875257599</v>
+        <v>-0.20000679900000001</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -47265,7 +47265,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <v>-0.158243137848496</v>
+        <v>-0.15824313800000001</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -47274,7 +47274,7 @@
         <v>1</v>
       </c>
       <c r="F42">
-        <v>0.111908260149312</v>
+        <v>0.11190826</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -47294,7 +47294,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <v>5.0048887465697002E-2</v>
+        <v>5.0048887E-2</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -47303,7 +47303,7 @@
         <v>1</v>
       </c>
       <c r="F43">
-        <v>9.6105461433904998E-2</v>
+        <v>9.6105461000000003E-2</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -47323,7 +47323,7 @@
         <v>1</v>
       </c>
       <c r="C44">
-        <v>-1.0987782431799999E-3</v>
+        <v>-1.0987779999999999E-3</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -47332,7 +47332,7 @@
         <v>1</v>
       </c>
       <c r="F44">
-        <v>-0.16801420274572801</v>
+        <v>-0.168014203</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -47352,7 +47352,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <v>-2.1298505576274E-2</v>
+        <v>-2.1298505999999998E-2</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -47361,7 +47361,7 @@
         <v>1</v>
       </c>
       <c r="F45">
-        <v>0.104505077199626</v>
+        <v>0.104505077</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -47381,7 +47381,7 @@
         <v>1</v>
       </c>
       <c r="C46">
-        <v>-2.2742302728967E-2</v>
+        <v>-2.2742302999999998E-2</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -47390,7 +47390,7 @@
         <v>1</v>
       </c>
       <c r="F46">
-        <v>0.19748212519772301</v>
+        <v>0.19748212500000001</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -47410,7 +47410,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <v>-1.7958159898718001E-2</v>
+        <v>-1.7958160000000001E-2</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -47419,7 +47419,7 @@
         <v>1</v>
       </c>
       <c r="F47">
-        <v>4.7172646144169002E-2</v>
+        <v>4.7172645999999999E-2</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -47439,7 +47439,7 @@
         <v>1</v>
       </c>
       <c r="C48">
-        <v>9.0683298523990003E-3</v>
+        <v>9.0683299999999994E-3</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -47448,7 +47448,7 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>2.975015604078E-3</v>
+        <v>2.975016E-3</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -47468,7 +47468,7 @@
         <v>1</v>
       </c>
       <c r="C49">
-        <v>9.9191179827126996E-2</v>
+        <v>9.9191180000000004E-2</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -47477,7 +47477,7 @@
         <v>1</v>
       </c>
       <c r="F49">
-        <v>5.3664149728770002E-3</v>
+        <v>5.3664150000000002E-3</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -47497,7 +47497,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>-0.15467363747655299</v>
+        <v>-0.154673637</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -47506,7 +47506,7 @@
         <v>0</v>
       </c>
       <c r="F50">
-        <v>-4.7245770833776998E-2</v>
+        <v>-4.7245770999999999E-2</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -47526,7 +47526,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <v>2.2147098518280998E-2</v>
+        <v>2.2147099E-2</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -47535,7 +47535,7 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <v>-0.186268714288958</v>
+        <v>-0.186268714</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -47555,7 +47555,7 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>-0.23911485899985599</v>
+        <v>-0.23911485900000001</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -47564,7 +47564,7 @@
         <v>1</v>
       </c>
       <c r="F52">
-        <v>-0.20115669735300201</v>
+        <v>-0.201156697</v>
       </c>
       <c r="G52">
         <v>1</v>
@@ -47584,7 +47584,7 @@
         <v>1</v>
       </c>
       <c r="C53">
-        <v>0.195881075636505</v>
+        <v>0.19588107599999999</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -47593,7 +47593,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>-0.155232369645563</v>
+        <v>-0.15523237000000001</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -47613,7 +47613,7 @@
         <v>0</v>
       </c>
       <c r="C54">
-        <v>-0.32695812747156</v>
+        <v>-0.32695812699999999</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -47622,7 +47622,7 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <v>-0.17377451139121</v>
+        <v>-0.17377451099999999</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -47642,7 +47642,7 @@
         <v>1</v>
       </c>
       <c r="C55">
-        <v>0.14970564601005701</v>
+        <v>0.149705646</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -47651,7 +47651,7 @@
         <v>1</v>
       </c>
       <c r="F55">
-        <v>-3.3679972290021003E-2</v>
+        <v>-3.3679972000000002E-2</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -47671,7 +47671,7 @@
         <v>0</v>
       </c>
       <c r="C56">
-        <v>-0.22534738651316399</v>
+        <v>-0.22534738700000001</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -47680,7 +47680,7 @@
         <v>1</v>
       </c>
       <c r="F56">
-        <v>0.13178104069579599</v>
+        <v>0.13178104099999999</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -47700,7 +47700,7 @@
         <v>1</v>
       </c>
       <c r="C57">
-        <v>0.178971213629049</v>
+        <v>0.17897121399999999</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -47709,7 +47709,7 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>-0.16706085153025299</v>
+        <v>-0.16706085200000001</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -47729,7 +47729,7 @@
         <v>0</v>
       </c>
       <c r="C58">
-        <v>-0.31884221907738802</v>
+        <v>-0.31884221899999998</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -47738,7 +47738,7 @@
         <v>1</v>
       </c>
       <c r="F58">
-        <v>-0.165501274133209</v>
+        <v>-0.165501274</v>
       </c>
       <c r="G58">
         <v>1</v>
@@ -47758,7 +47758,7 @@
         <v>1</v>
       </c>
       <c r="C59">
-        <v>0.26413236238451898</v>
+        <v>0.26413236200000001</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -47767,7 +47767,7 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>-0.23643970322416499</v>
+        <v>-0.236439703</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -47787,7 +47787,7 @@
         <v>0</v>
       </c>
       <c r="C60">
-        <v>-0.15230453275990699</v>
+        <v>-0.15230453299999999</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -47796,7 +47796,7 @@
         <v>1</v>
       </c>
       <c r="F60">
-        <v>0.11652699414513</v>
+        <v>0.11652699399999999</v>
       </c>
       <c r="G60">
         <v>1</v>
@@ -47816,7 +47816,7 @@
         <v>1</v>
       </c>
       <c r="C61">
-        <v>0.16030939167928199</v>
+        <v>0.160309392</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -47825,7 +47825,7 @@
         <v>1</v>
       </c>
       <c r="F61">
-        <v>0.21964416896979699</v>
+        <v>0.219644169</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -47845,7 +47845,7 @@
         <v>0</v>
       </c>
       <c r="C62">
-        <v>-0.14666354559832201</v>
+        <v>-0.14666354600000001</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -47854,7 +47854,7 @@
         <v>1</v>
       </c>
       <c r="F62">
-        <v>0.122210050239013</v>
+        <v>0.12221005</v>
       </c>
       <c r="G62">
         <v>1</v>
@@ -47874,7 +47874,7 @@
         <v>0</v>
       </c>
       <c r="C63">
-        <v>-1.0437161274953999E-2</v>
+        <v>-1.0437161E-2</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -47883,7 +47883,7 @@
         <v>1</v>
       </c>
       <c r="F63">
-        <v>-9.8879019474089995E-3</v>
+        <v>-9.8879020000000005E-3</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -47903,7 +47903,7 @@
         <v>0</v>
       </c>
       <c r="C64">
-        <v>-0.26462168388531299</v>
+        <v>-0.26462168400000002</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -47912,7 +47912,7 @@
         <v>1</v>
       </c>
       <c r="F64">
-        <v>-0.102125441669681</v>
+        <v>-0.102125442</v>
       </c>
       <c r="G64">
         <v>1</v>
@@ -47932,7 +47932,7 @@
         <v>1</v>
       </c>
       <c r="C65">
-        <v>2.4863030131543E-2</v>
+        <v>2.4863030000000001E-2</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -47941,7 +47941,7 @@
         <v>0</v>
       </c>
       <c r="F65">
-        <v>-0.180333208606306</v>
+        <v>-0.18033320899999999</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -47961,7 +47961,7 @@
         <v>0</v>
       </c>
       <c r="C66">
-        <v>-0.21388553958238499</v>
+        <v>-0.21388554000000001</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -47970,7 +47970,7 @@
         <v>1</v>
       </c>
       <c r="F66">
-        <v>0.152360403075014</v>
+        <v>0.15236040300000001</v>
       </c>
       <c r="G66">
         <v>1</v>
@@ -47990,7 +47990,7 @@
         <v>1</v>
       </c>
       <c r="C67">
-        <v>0.20452021866669801</v>
+        <v>0.204520219</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -47999,7 +47999,7 @@
         <v>1</v>
       </c>
       <c r="F67">
-        <v>0.33607513888757701</v>
+        <v>0.33607513900000002</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -48019,7 +48019,7 @@
         <v>0</v>
       </c>
       <c r="C68">
-        <v>-0.22066273492487001</v>
+        <v>-0.220662735</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -48028,7 +48028,7 @@
         <v>1</v>
       </c>
       <c r="F68">
-        <v>0.180597958035697</v>
+        <v>0.180597958</v>
       </c>
       <c r="G68">
         <v>1</v>
@@ -48048,7 +48048,7 @@
         <v>1</v>
       </c>
       <c r="C69">
-        <v>0.19438320462268299</v>
+        <v>0.194383205</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -48057,7 +48057,7 @@
         <v>0</v>
       </c>
       <c r="F69">
-        <v>-0.173755922781717</v>
+        <v>-0.17375592300000001</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -48077,7 +48077,7 @@
         <v>0</v>
       </c>
       <c r="C70">
-        <v>-0.22148123999986</v>
+        <v>-0.22148124</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -48086,7 +48086,7 @@
         <v>1</v>
       </c>
       <c r="F70">
-        <v>0.20591398512725101</v>
+        <v>0.20591398499999999</v>
       </c>
       <c r="G70">
         <v>1</v>
@@ -48106,7 +48106,7 @@
         <v>1</v>
       </c>
       <c r="C71">
-        <v>0.18794673141535501</v>
+        <v>0.18794673100000001</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -48115,7 +48115,7 @@
         <v>0</v>
       </c>
       <c r="F71">
-        <v>-0.157780328773786</v>
+        <v>-0.157780329</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -48135,7 +48135,7 @@
         <v>0</v>
       </c>
       <c r="C72">
-        <v>-0.183413759454363</v>
+        <v>-0.18341375900000001</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -48144,7 +48144,7 @@
         <v>1</v>
       </c>
       <c r="F72">
-        <v>-0.178745346212309</v>
+        <v>-0.178745346</v>
       </c>
       <c r="G72">
         <v>1</v>
@@ -48164,7 +48164,7 @@
         <v>1</v>
       </c>
       <c r="C73">
-        <v>0.18923781301245199</v>
+        <v>0.189237813</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -48173,7 +48173,7 @@
         <v>1</v>
       </c>
       <c r="F73">
-        <v>-5.1790508429324998E-2</v>
+        <v>-5.1790507999999999E-2</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -48193,7 +48193,7 @@
         <v>0</v>
       </c>
       <c r="C74">
-        <v>-0.273604179944134</v>
+        <v>-0.27360417999999997</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -48202,7 +48202,7 @@
         <v>1</v>
       </c>
       <c r="F74">
-        <v>-0.11538044445569499</v>
+        <v>-0.115380444</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -48222,7 +48222,7 @@
         <v>1</v>
       </c>
       <c r="C75">
-        <v>0.14208321723940401</v>
+        <v>0.14208321700000001</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -48231,7 +48231,7 @@
         <v>0</v>
       </c>
       <c r="F75">
-        <v>-0.120323807673319</v>
+        <v>-0.120323808</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -48251,7 +48251,7 @@
         <v>0</v>
       </c>
       <c r="C76">
-        <v>-0.15704346654469301</v>
+        <v>-0.15704346699999999</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -48260,7 +48260,7 @@
         <v>0</v>
       </c>
       <c r="F76">
-        <v>-1.2915638632419999E-3</v>
+        <v>-1.291564E-3</v>
       </c>
       <c r="G76">
         <v>1</v>
@@ -48280,7 +48280,7 @@
         <v>1</v>
       </c>
       <c r="C77">
-        <v>-1.6539689583644001E-2</v>
+        <v>-1.6539689999999999E-2</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -48289,7 +48289,7 @@
         <v>1</v>
       </c>
       <c r="F77">
-        <v>6.2588791318209006E-2</v>
+        <v>6.2588791000000005E-2</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -48309,7 +48309,7 @@
         <v>0</v>
       </c>
       <c r="C78">
-        <v>-0.35615409716945001</v>
+        <v>-0.356154097</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -48318,7 +48318,7 @@
         <v>1</v>
       </c>
       <c r="F78">
-        <v>0.131278260351746</v>
+        <v>0.13127826000000001</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -48338,7 +48338,7 @@
         <v>1</v>
       </c>
       <c r="C79">
-        <v>0.161271240962439</v>
+        <v>0.16127124100000001</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -48347,7 +48347,7 @@
         <v>0</v>
       </c>
       <c r="F79">
-        <v>-0.142186471082515</v>
+        <v>-0.14218647100000001</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -48367,7 +48367,7 @@
         <v>1</v>
       </c>
       <c r="C80">
-        <v>5.3208037610046E-2</v>
+        <v>5.3208037999999999E-2</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -48376,7 +48376,7 @@
         <v>1</v>
       </c>
       <c r="F80">
-        <v>1.0223984287827E-2</v>
+        <v>1.0223984E-2</v>
       </c>
       <c r="G80">
         <v>1</v>
@@ -48396,7 +48396,7 @@
         <v>1</v>
       </c>
       <c r="C81">
-        <v>0.105092369665734</v>
+        <v>0.10509237</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -48405,7 +48405,7 @@
         <v>1</v>
       </c>
       <c r="F81">
-        <v>-1.2818413329636E-2</v>
+        <v>-1.2818413000000001E-2</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -48425,7 +48425,7 @@
         <v>0</v>
       </c>
       <c r="C82">
-        <v>-0.10201137287809001</v>
+        <v>-0.102011373</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -48434,7 +48434,7 @@
         <v>1</v>
       </c>
       <c r="F82">
-        <v>9.7624352778300004E-4</v>
+        <v>9.7624400000000003E-4</v>
       </c>
       <c r="G82">
         <v>1</v>
@@ -48454,7 +48454,7 @@
         <v>1</v>
       </c>
       <c r="C83">
-        <v>0.11757172801388099</v>
+        <v>0.117571728</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -48463,7 +48463,7 @@
         <v>0</v>
       </c>
       <c r="F83">
-        <v>3.7730149618120002E-3</v>
+        <v>3.7730149999999998E-3</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -48483,7 +48483,7 @@
         <v>0</v>
       </c>
       <c r="C84">
-        <v>-0.15918113453205801</v>
+        <v>-0.159181135</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -48492,7 +48492,7 @@
         <v>1</v>
       </c>
       <c r="F84">
-        <v>0.11313383398636601</v>
+        <v>0.113133834</v>
       </c>
       <c r="G84">
         <v>1</v>
@@ -48512,7 +48512,7 @@
         <v>1</v>
       </c>
       <c r="C85">
-        <v>0.122697982367105</v>
+        <v>0.122697982</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -48521,7 +48521,7 @@
         <v>0</v>
       </c>
       <c r="F85">
-        <v>-0.13366200806164999</v>
+        <v>-0.133662008</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -48541,7 +48541,7 @@
         <v>0</v>
       </c>
       <c r="C86">
-        <v>-0.115999808439659</v>
+        <v>-0.115999808</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -48550,7 +48550,7 @@
         <v>1</v>
       </c>
       <c r="F86">
-        <v>0.139786711099712</v>
+        <v>0.13978671100000001</v>
       </c>
       <c r="G86">
         <v>1</v>
@@ -48570,7 +48570,7 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>0.16345198403401401</v>
+        <v>0.16345198399999999</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -48579,7 +48579,7 @@
         <v>1</v>
       </c>
       <c r="F87">
-        <v>-3.8748227954689997E-2</v>
+        <v>-3.8748228000000003E-2</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -48599,7 +48599,7 @@
         <v>0</v>
       </c>
       <c r="C88">
-        <v>-0.13991393499259799</v>
+        <v>-0.13991393499999999</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -48608,7 +48608,7 @@
         <v>1</v>
       </c>
       <c r="F88">
-        <v>0.162419218849611</v>
+        <v>0.162419219</v>
       </c>
       <c r="G88">
         <v>1</v>
@@ -48628,7 +48628,7 @@
         <v>1</v>
       </c>
       <c r="C89">
-        <v>9.3064281274971003E-2</v>
+        <v>9.3064280999999999E-2</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -48637,7 +48637,7 @@
         <v>0</v>
       </c>
       <c r="F89">
-        <v>-0.108765002620727</v>
+        <v>-0.108765003</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -48657,7 +48657,7 @@
         <v>0</v>
       </c>
       <c r="C90">
-        <v>-0.11062642586065401</v>
+        <v>-0.110626426</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -48666,7 +48666,7 @@
         <v>1</v>
       </c>
       <c r="F90">
-        <v>-2.8282894996770002E-3</v>
+        <v>-2.8282889999999999E-3</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -48686,7 +48686,7 @@
         <v>1</v>
       </c>
       <c r="C91">
-        <v>-2.0699391527400001E-3</v>
+        <v>-2.0699389999999998E-3</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -48695,7 +48695,7 @@
         <v>0</v>
       </c>
       <c r="F91">
-        <v>-0.113837512095641</v>
+        <v>-0.113837512</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -48715,7 +48715,7 @@
         <v>0</v>
       </c>
       <c r="C92">
-        <v>-0.17824162871940299</v>
+        <v>-0.17824162900000001</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -48724,7 +48724,7 @@
         <v>1</v>
       </c>
       <c r="F92">
-        <v>-5.4817109746539998E-3</v>
+        <v>-5.4817110000000002E-3</v>
       </c>
       <c r="G92">
         <v>1</v>
@@ -48744,7 +48744,7 @@
         <v>1</v>
       </c>
       <c r="C93">
-        <v>0.13189551887155701</v>
+        <v>0.13189551899999999</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -48753,7 +48753,7 @@
         <v>1</v>
       </c>
       <c r="F93">
-        <v>7.6402326949309998E-2</v>
+        <v>7.6402327000000006E-2</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -48773,7 +48773,7 @@
         <v>0</v>
       </c>
       <c r="C94">
-        <v>-0.123514009213835</v>
+        <v>-0.12351400899999999</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -48782,7 +48782,7 @@
         <v>1</v>
       </c>
       <c r="F94">
-        <v>0.12191299153200701</v>
+        <v>0.121912992</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -48802,7 +48802,7 @@
         <v>1</v>
       </c>
       <c r="C95">
-        <v>0.10540591574715499</v>
+        <v>0.105405916</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -48811,7 +48811,7 @@
         <v>0</v>
       </c>
       <c r="F95">
-        <v>-1.6821573163617001E-2</v>
+        <v>-1.6821572999999999E-2</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -48831,7 +48831,7 @@
         <v>1</v>
       </c>
       <c r="C96">
-        <v>3.6931581275430003E-2</v>
+        <v>3.6931580999999998E-2</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -48840,7 +48840,7 @@
         <v>1</v>
       </c>
       <c r="F96">
-        <v>3.2453022433112003E-2</v>
+        <v>3.2453021999999998E-2</v>
       </c>
       <c r="G96">
         <v>1</v>
@@ -48860,7 +48860,7 @@
         <v>1</v>
       </c>
       <c r="C97">
-        <v>0.10899648432013399</v>
+        <v>0.108996484</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -48869,7 +48869,7 @@
         <v>1</v>
       </c>
       <c r="F97">
-        <v>8.2320292079367002E-2</v>
+        <v>8.2320292000000003E-2</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -48889,7 +48889,7 @@
         <v>0</v>
       </c>
       <c r="C98">
-        <v>-9.7046751234984005E-2</v>
+        <v>-9.7046751000000001E-2</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -48898,7 +48898,7 @@
         <v>1</v>
       </c>
       <c r="F98">
-        <v>3.3825510797829998E-3</v>
+        <v>3.3825510000000001E-3</v>
       </c>
       <c r="G98">
         <v>1</v>
@@ -48918,7 +48918,7 @@
         <v>1</v>
       </c>
       <c r="C99">
-        <v>0.178687757762445</v>
+        <v>0.178687758</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -48927,7 +48927,7 @@
         <v>0</v>
       </c>
       <c r="F99">
-        <v>-1.3051369501976001E-2</v>
+        <v>-1.305137E-2</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -48947,7 +48947,7 @@
         <v>0</v>
       </c>
       <c r="C100">
-        <v>-0.119347291889037</v>
+        <v>-0.11934729199999999</v>
       </c>
       <c r="D100">
         <v>1</v>
@@ -48956,7 +48956,7 @@
         <v>1</v>
       </c>
       <c r="F100">
-        <v>6.2206800287199998E-4</v>
+        <v>6.2206800000000003E-4</v>
       </c>
       <c r="G100">
         <v>1</v>
@@ -48976,7 +48976,7 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>0.15011198786749899</v>
+        <v>0.150111988</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -48985,7 +48985,7 @@
         <v>0</v>
       </c>
       <c r="F101">
-        <v>-1.1652436904024E-2</v>
+        <v>-1.1652437E-2</v>
       </c>
       <c r="G101">
         <v>1</v>
@@ -49005,7 +49005,7 @@
         <v>1</v>
       </c>
       <c r="C102">
-        <v>6.6583278160225995E-2</v>
+        <v>6.6583277999999996E-2</v>
       </c>
       <c r="D102">
         <v>1</v>
@@ -49014,7 +49014,7 @@
         <v>1</v>
       </c>
       <c r="F102">
-        <v>8.4979370741900002E-3</v>
+        <v>8.4979370000000005E-3</v>
       </c>
       <c r="G102">
         <v>1</v>
@@ -49034,7 +49034,7 @@
         <v>0</v>
       </c>
       <c r="C103">
-        <v>-0.53317081973829294</v>
+        <v>-0.53317082000000005</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -49043,7 +49043,7 @@
         <v>1</v>
       </c>
       <c r="F103">
-        <v>0.418776847215315</v>
+        <v>0.41877684700000001</v>
       </c>
       <c r="G103">
         <v>1</v>
@@ -49063,7 +49063,7 @@
         <v>1</v>
       </c>
       <c r="C104">
-        <v>0.174486684852629</v>
+        <v>0.174486685</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -49072,7 +49072,7 @@
         <v>0</v>
       </c>
       <c r="F104">
-        <v>-0.11983927625103701</v>
+        <v>-0.11983927599999999</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -49092,7 +49092,7 @@
         <v>0</v>
       </c>
       <c r="C105">
-        <v>-0.110900906428491</v>
+        <v>-0.11090090599999999</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -49101,7 +49101,7 @@
         <v>1</v>
       </c>
       <c r="F105">
-        <v>0.12530896079849899</v>
+        <v>0.125308961</v>
       </c>
       <c r="G105">
         <v>1</v>
@@ -49121,7 +49121,7 @@
         <v>0</v>
       </c>
       <c r="C106">
-        <v>-3.1255364625172997E-2</v>
+        <v>-3.1255365E-2</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -49130,7 +49130,7 @@
         <v>1</v>
       </c>
       <c r="F106">
-        <v>8.3356723436002006E-2</v>
+        <v>8.3356722999999994E-2</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -49150,7 +49150,7 @@
         <v>0</v>
       </c>
       <c r="C107">
-        <v>0.19486796385866001</v>
+        <v>0.194867964</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -49159,7 +49159,7 @@
         <v>1</v>
       </c>
       <c r="F107">
-        <v>0.48492690087323098</v>
+        <v>0.48492690100000002</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -49179,7 +49179,7 @@
         <v>0</v>
       </c>
       <c r="C108">
-        <v>-0.60077377795770504</v>
+        <v>-0.60077377799999998</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -49188,7 +49188,7 @@
         <v>0</v>
       </c>
       <c r="F108">
-        <v>-0.237123487019715</v>
+        <v>-0.23712348699999999</v>
       </c>
       <c r="G108">
         <v>1</v>
@@ -49208,7 +49208,7 @@
         <v>0</v>
       </c>
       <c r="C109">
-        <v>1.1669641101446001E-2</v>
+        <v>1.1669641E-2</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -49217,7 +49217,7 @@
         <v>1</v>
       </c>
       <c r="F109">
-        <v>-2.2932818099174999E-2</v>
+        <v>-2.2932818000000001E-2</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -49237,7 +49237,7 @@
         <v>0</v>
       </c>
       <c r="C110">
-        <v>-0.15566774087615901</v>
+        <v>-0.155667741</v>
       </c>
       <c r="D110">
         <v>0</v>
@@ -49246,7 +49246,7 @@
         <v>1</v>
       </c>
       <c r="F110">
-        <v>0.108522311265966</v>
+        <v>0.108522311</v>
       </c>
       <c r="G110">
         <v>1</v>
@@ -49266,7 +49266,7 @@
         <v>0</v>
       </c>
       <c r="C111">
-        <v>4.7832708928762999E-2</v>
+        <v>4.7832709000000001E-2</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -49275,7 +49275,7 @@
         <v>0</v>
       </c>
       <c r="F111">
-        <v>-0.107807582326715</v>
+        <v>-0.107807582</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -49295,7 +49295,7 @@
         <v>0</v>
       </c>
       <c r="C112">
-        <v>-0.117697529359594</v>
+        <v>-0.117697529</v>
       </c>
       <c r="D112">
         <v>1</v>
@@ -49304,7 +49304,7 @@
         <v>1</v>
       </c>
       <c r="F112">
-        <v>-2.4182710563851E-2</v>
+        <v>-2.4182710999999999E-2</v>
       </c>
       <c r="G112">
         <v>1</v>
@@ -49324,7 +49324,7 @@
         <v>1</v>
       </c>
       <c r="C113">
-        <v>0.18737942908371399</v>
+        <v>0.18737942899999999</v>
       </c>
       <c r="D113">
         <v>1</v>
@@ -49333,7 +49333,7 @@
         <v>1</v>
       </c>
       <c r="F113">
-        <v>-4.7641643289103003E-2</v>
+        <v>-4.7641642999999997E-2</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -49353,7 +49353,7 @@
         <v>0</v>
       </c>
       <c r="C114">
-        <v>-0.124133860307092</v>
+        <v>-0.12413386</v>
       </c>
       <c r="D114">
         <v>1</v>
@@ -49362,7 +49362,7 @@
         <v>1</v>
       </c>
       <c r="F114">
-        <v>-0.121484781558247</v>
+        <v>-0.121484782</v>
       </c>
       <c r="G114">
         <v>1</v>
@@ -49382,7 +49382,7 @@
         <v>1</v>
       </c>
       <c r="C115">
-        <v>0.15927304427733399</v>
+        <v>0.159273044</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -49391,7 +49391,7 @@
         <v>1</v>
       </c>
       <c r="F115">
-        <v>9.3392892195125005E-2</v>
+        <v>9.3392892000000005E-2</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -49411,7 +49411,7 @@
         <v>1</v>
       </c>
       <c r="C116">
-        <v>8.6727100335694002E-2</v>
+        <v>8.6727100000000001E-2</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -49420,7 +49420,7 @@
         <v>1</v>
       </c>
       <c r="F116">
-        <v>0.143856197150079</v>
+        <v>0.14385619699999999</v>
       </c>
       <c r="G116">
         <v>1</v>
@@ -49440,7 +49440,7 @@
         <v>1</v>
       </c>
       <c r="C117">
-        <v>0.20847652484180801</v>
+        <v>0.208476525</v>
       </c>
       <c r="D117">
         <v>0</v>
@@ -49449,7 +49449,7 @@
         <v>1</v>
       </c>
       <c r="F117">
-        <v>0.105892009059274</v>
+        <v>0.105892009</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -49469,7 +49469,7 @@
         <v>0</v>
       </c>
       <c r="C118">
-        <v>-0.112755145241889</v>
+        <v>-0.112755145</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -49478,7 +49478,7 @@
         <v>1</v>
       </c>
       <c r="F118">
-        <v>0.11334380622228001</v>
+        <v>0.11334380600000001</v>
       </c>
       <c r="G118">
         <v>1</v>
@@ -49498,7 +49498,7 @@
         <v>1</v>
       </c>
       <c r="C119">
-        <v>0.1171300247188</v>
+        <v>0.117130025</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -49507,7 +49507,7 @@
         <v>0</v>
       </c>
       <c r="F119">
-        <v>9.0801119993489995E-3</v>
+        <v>9.0801119999999996E-3</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -49527,7 +49527,7 @@
         <v>0</v>
       </c>
       <c r="C120">
-        <v>-0.11972002909356901</v>
+        <v>-0.11972002900000001</v>
       </c>
       <c r="D120">
         <v>1</v>
@@ -49536,7 +49536,7 @@
         <v>0</v>
       </c>
       <c r="F120">
-        <v>-6.3879275043950995E-2</v>
+        <v>-6.3879274999999999E-2</v>
       </c>
       <c r="G120">
         <v>1</v>
@@ -49556,7 +49556,7 @@
         <v>1</v>
       </c>
       <c r="C121">
-        <v>0.12982867431265299</v>
+        <v>0.12982867400000001</v>
       </c>
       <c r="D121">
         <v>1</v>
@@ -49565,7 +49565,7 @@
         <v>0</v>
       </c>
       <c r="F121">
-        <v>-0.11189895173039401</v>
+        <v>-0.111898952</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -49575,6 +49575,2587 @@
       </c>
       <c r="I121" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>1</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+      <c r="C122">
+        <v>-0.192599603290801</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>1</v>
+      </c>
+      <c r="F122">
+        <v>0.149453614155974</v>
+      </c>
+      <c r="G122">
+        <v>1</v>
+      </c>
+      <c r="H122">
+        <v>1</v>
+      </c>
+      <c r="I122" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>0</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+      <c r="C123">
+        <v>4.5895041596461003E-2</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123">
+        <v>1</v>
+      </c>
+      <c r="F123">
+        <v>0.309895358031478</v>
+      </c>
+      <c r="G123">
+        <v>0</v>
+      </c>
+      <c r="H123">
+        <v>1</v>
+      </c>
+      <c r="I123" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>1</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+      <c r="C124">
+        <v>-0.207466539852243</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="E124">
+        <v>1</v>
+      </c>
+      <c r="F124">
+        <v>0.16404748688027601</v>
+      </c>
+      <c r="G124">
+        <v>1</v>
+      </c>
+      <c r="H124">
+        <v>1</v>
+      </c>
+      <c r="I124" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>0</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+      <c r="C125">
+        <v>0.130917065004518</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <v>-0.26360674197705602</v>
+      </c>
+      <c r="G125">
+        <v>1</v>
+      </c>
+      <c r="H125">
+        <v>0</v>
+      </c>
+      <c r="I125" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>1</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="C126">
+        <v>-0.29348461896359901</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+      <c r="E126">
+        <v>1</v>
+      </c>
+      <c r="F126">
+        <v>-0.120954367298072</v>
+      </c>
+      <c r="G126">
+        <v>0</v>
+      </c>
+      <c r="H126">
+        <v>0</v>
+      </c>
+      <c r="I126" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>1</v>
+      </c>
+      <c r="B127">
+        <v>0</v>
+      </c>
+      <c r="C127">
+        <v>-0.48191736511646499</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127">
+        <v>1</v>
+      </c>
+      <c r="F127">
+        <v>-0.17465350445651701</v>
+      </c>
+      <c r="G127">
+        <v>0</v>
+      </c>
+      <c r="H127">
+        <v>0</v>
+      </c>
+      <c r="I127" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>0</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="C128">
+        <v>0.34695775395133899</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <v>-0.29891169453785299</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+      <c r="H128">
+        <v>1</v>
+      </c>
+      <c r="I128" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>1</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+      <c r="C129">
+        <v>-0.21147035255465199</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <v>-0.79124143043642703</v>
+      </c>
+      <c r="G129">
+        <v>1</v>
+      </c>
+      <c r="H129">
+        <v>0</v>
+      </c>
+      <c r="I129" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>0</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130">
+        <v>0.27764796855316498</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="E130">
+        <v>1</v>
+      </c>
+      <c r="F130">
+        <v>0.19764193052913701</v>
+      </c>
+      <c r="G130">
+        <v>1</v>
+      </c>
+      <c r="H130">
+        <v>0</v>
+      </c>
+      <c r="I130" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>1</v>
+      </c>
+      <c r="B131">
+        <v>0</v>
+      </c>
+      <c r="C131">
+        <v>-0.13392549323330899</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <v>-0.123380724352608</v>
+      </c>
+      <c r="G131">
+        <v>1</v>
+      </c>
+      <c r="H131">
+        <v>1</v>
+      </c>
+      <c r="I131" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>0</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+      <c r="C132">
+        <v>0.21905243101098101</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="F132">
+        <v>0.177717760725879</v>
+      </c>
+      <c r="G132">
+        <v>1</v>
+      </c>
+      <c r="H132">
+        <v>1</v>
+      </c>
+      <c r="I132" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>1</v>
+      </c>
+      <c r="B133">
+        <v>0</v>
+      </c>
+      <c r="C133">
+        <v>-0.237217916007639</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+      <c r="E133">
+        <v>1</v>
+      </c>
+      <c r="F133">
+        <v>-0.126598876372815</v>
+      </c>
+      <c r="G133">
+        <v>0</v>
+      </c>
+      <c r="H133">
+        <v>0</v>
+      </c>
+      <c r="I133" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>1</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134">
+        <v>8.8115238945699996E-3</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+      <c r="E134">
+        <v>0</v>
+      </c>
+      <c r="F134">
+        <v>-0.26444634331843703</v>
+      </c>
+      <c r="G134">
+        <v>0</v>
+      </c>
+      <c r="H134">
+        <v>1</v>
+      </c>
+      <c r="I134" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>1</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+      <c r="C135">
+        <v>-0.25596241663328601</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+      <c r="E135">
+        <v>1</v>
+      </c>
+      <c r="F135">
+        <v>-0.116237686543126</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
+      <c r="H135">
+        <v>0</v>
+      </c>
+      <c r="I135" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>0</v>
+      </c>
+      <c r="B136">
+        <v>0</v>
+      </c>
+      <c r="C136">
+        <v>-1.5325040631473E-2</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+      <c r="F136">
+        <v>1.08373655535008</v>
+      </c>
+      <c r="G136">
+        <v>1</v>
+      </c>
+      <c r="H136">
+        <v>0</v>
+      </c>
+      <c r="I136" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>1</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+      <c r="C137">
+        <v>-0.25456139810515799</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <v>-0.60184683225587099</v>
+      </c>
+      <c r="G137">
+        <v>1</v>
+      </c>
+      <c r="H137">
+        <v>0</v>
+      </c>
+      <c r="I137" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>0</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+      <c r="C138">
+        <v>0.18462639863073599</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+      <c r="F138">
+        <v>0.283468285472322</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
+      <c r="H138">
+        <v>0</v>
+      </c>
+      <c r="I138" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>1</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+      <c r="C139">
+        <v>-0.14819440236291501</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139">
+        <v>-0.61864327696256405</v>
+      </c>
+      <c r="G139">
+        <v>1</v>
+      </c>
+      <c r="H139">
+        <v>0</v>
+      </c>
+      <c r="I139" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>0</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+      <c r="C140">
+        <v>3.2164030288606003E-2</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140">
+        <v>2.8029395818391999E-2</v>
+      </c>
+      <c r="G140">
+        <v>1</v>
+      </c>
+      <c r="H140">
+        <v>0</v>
+      </c>
+      <c r="I140" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>1</v>
+      </c>
+      <c r="B141">
+        <v>0</v>
+      </c>
+      <c r="C141">
+        <v>-0.16225957973203001</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>1</v>
+      </c>
+      <c r="F141">
+        <v>0.16016923155254301</v>
+      </c>
+      <c r="G141">
+        <v>0</v>
+      </c>
+      <c r="H141">
+        <v>1</v>
+      </c>
+      <c r="I141" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>0</v>
+      </c>
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="C142">
+        <v>0.22381711250113701</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142">
+        <v>-0.109761199398207</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+      <c r="H142">
+        <v>1</v>
+      </c>
+      <c r="I142" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>1</v>
+      </c>
+      <c r="B143">
+        <v>0</v>
+      </c>
+      <c r="C143">
+        <v>-0.13298007635433701</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <v>-6.820967720427E-2</v>
+      </c>
+      <c r="G143">
+        <v>1</v>
+      </c>
+      <c r="H143">
+        <v>1</v>
+      </c>
+      <c r="I143" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>1</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
+      <c r="C144">
+        <v>2.0265851853149999E-3</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144">
+        <v>-0.132408438282172</v>
+      </c>
+      <c r="G144">
+        <v>1</v>
+      </c>
+      <c r="H144">
+        <v>0</v>
+      </c>
+      <c r="I144" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>1</v>
+      </c>
+      <c r="B145">
+        <v>0</v>
+      </c>
+      <c r="C145">
+        <v>-0.13842122716859001</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145">
+        <v>-0.36972641671052697</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145">
+        <v>1</v>
+      </c>
+      <c r="I145" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>1</v>
+      </c>
+      <c r="B146">
+        <v>0</v>
+      </c>
+      <c r="C146">
+        <v>-0.245517419683284</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
+      <c r="F146">
+        <v>0.451238699713709</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+      <c r="H146">
+        <v>1</v>
+      </c>
+      <c r="I146" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>1</v>
+      </c>
+      <c r="B147">
+        <v>0</v>
+      </c>
+      <c r="C147">
+        <v>-0.24518203014954101</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147">
+        <v>-0.48927308785826301</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+      <c r="H147">
+        <v>1</v>
+      </c>
+      <c r="I147" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>0</v>
+      </c>
+      <c r="B148">
+        <v>0</v>
+      </c>
+      <c r="C148">
+        <v>3.2318329080224001E-2</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148">
+        <v>-0.26105390530214401</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+      <c r="H148">
+        <v>0</v>
+      </c>
+      <c r="I148" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>1</v>
+      </c>
+      <c r="B149">
+        <v>0</v>
+      </c>
+      <c r="C149">
+        <v>-0.15746835577742399</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+      <c r="F149">
+        <v>-0.39468212879065601</v>
+      </c>
+      <c r="G149">
+        <v>1</v>
+      </c>
+      <c r="H149">
+        <v>0</v>
+      </c>
+      <c r="I149" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>0</v>
+      </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
+      <c r="C150">
+        <v>0.84551350116701196</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150">
+        <v>1</v>
+      </c>
+      <c r="F150">
+        <v>0.239101487308127</v>
+      </c>
+      <c r="G150">
+        <v>0</v>
+      </c>
+      <c r="H150">
+        <v>1</v>
+      </c>
+      <c r="I150" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>1</v>
+      </c>
+      <c r="B151">
+        <v>0</v>
+      </c>
+      <c r="C151">
+        <v>-0.19129599769761799</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="F151">
+        <v>0.16991034066292601</v>
+      </c>
+      <c r="G151">
+        <v>1</v>
+      </c>
+      <c r="H151">
+        <v>1</v>
+      </c>
+      <c r="I151" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>1</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <v>-0.26795982009499397</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+      <c r="E152">
+        <v>1</v>
+      </c>
+      <c r="F152">
+        <v>0.40460682240590901</v>
+      </c>
+      <c r="G152">
+        <v>0</v>
+      </c>
+      <c r="H152">
+        <v>1</v>
+      </c>
+      <c r="I152" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>1</v>
+      </c>
+      <c r="B153">
+        <v>0</v>
+      </c>
+      <c r="C153">
+        <v>-0.41834517404687899</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="F153">
+        <v>-0.20805827870947399</v>
+      </c>
+      <c r="G153">
+        <v>0</v>
+      </c>
+      <c r="H153">
+        <v>1</v>
+      </c>
+      <c r="I153" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>1</v>
+      </c>
+      <c r="B154">
+        <v>0</v>
+      </c>
+      <c r="C154">
+        <v>-0.23040601931850499</v>
+      </c>
+      <c r="D154">
+        <v>1</v>
+      </c>
+      <c r="E154">
+        <v>1</v>
+      </c>
+      <c r="F154">
+        <v>0.14951990027008599</v>
+      </c>
+      <c r="G154">
+        <v>0</v>
+      </c>
+      <c r="H154">
+        <v>0</v>
+      </c>
+      <c r="I154" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>1</v>
+      </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
+      <c r="C155">
+        <v>-0.33335862766697599</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
+      </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
+      <c r="F155">
+        <v>-0.63587457077132803</v>
+      </c>
+      <c r="G155">
+        <v>0</v>
+      </c>
+      <c r="H155">
+        <v>0</v>
+      </c>
+      <c r="I155" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>0</v>
+      </c>
+      <c r="B156">
+        <v>0</v>
+      </c>
+      <c r="C156">
+        <v>0.193834242737912</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+      <c r="F156">
+        <v>4.9612358312254003E-2</v>
+      </c>
+      <c r="G156">
+        <v>1</v>
+      </c>
+      <c r="H156">
+        <v>1</v>
+      </c>
+      <c r="I156" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>1</v>
+      </c>
+      <c r="B157">
+        <v>0</v>
+      </c>
+      <c r="C157">
+        <v>-0.14990811136854101</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157">
+        <v>-0.12629773605129099</v>
+      </c>
+      <c r="G157">
+        <v>1</v>
+      </c>
+      <c r="H157">
+        <v>1</v>
+      </c>
+      <c r="I157" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>0</v>
+      </c>
+      <c r="B158">
+        <v>0</v>
+      </c>
+      <c r="C158">
+        <v>0.30143592146320503</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
+      <c r="F158">
+        <v>0.21627892960981501</v>
+      </c>
+      <c r="G158">
+        <v>1</v>
+      </c>
+      <c r="H158">
+        <v>1</v>
+      </c>
+      <c r="I158" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>1</v>
+      </c>
+      <c r="B159">
+        <v>0</v>
+      </c>
+      <c r="C159">
+        <v>-0.37444725341665003</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="F159">
+        <v>-0.64386080623515096</v>
+      </c>
+      <c r="G159">
+        <v>0</v>
+      </c>
+      <c r="H159">
+        <v>0</v>
+      </c>
+      <c r="I159" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>1</v>
+      </c>
+      <c r="B160">
+        <v>0</v>
+      </c>
+      <c r="C160">
+        <v>-0.243173453404054</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+      <c r="E160">
+        <v>1</v>
+      </c>
+      <c r="F160">
+        <v>3.1294442438073999E-2</v>
+      </c>
+      <c r="G160">
+        <v>0</v>
+      </c>
+      <c r="H160">
+        <v>1</v>
+      </c>
+      <c r="I160" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>1</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>-0.32228136804910201</v>
+      </c>
+      <c r="D161">
+        <v>0</v>
+      </c>
+      <c r="E161">
+        <v>0</v>
+      </c>
+      <c r="F161">
+        <v>-0.184224726862496</v>
+      </c>
+      <c r="G161">
+        <v>0</v>
+      </c>
+      <c r="H161">
+        <v>0</v>
+      </c>
+      <c r="I161" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>1</v>
+      </c>
+      <c r="B162">
+        <v>0</v>
+      </c>
+      <c r="C162">
+        <v>-0.249575801003345</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+      <c r="E162">
+        <v>1</v>
+      </c>
+      <c r="F162">
+        <v>0.18224649776319199</v>
+      </c>
+      <c r="G162">
+        <v>0</v>
+      </c>
+      <c r="H162">
+        <v>1</v>
+      </c>
+      <c r="I162" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>1</v>
+      </c>
+      <c r="B163">
+        <v>0</v>
+      </c>
+      <c r="C163">
+        <v>-0.14818888840837499</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+      <c r="E163">
+        <v>0</v>
+      </c>
+      <c r="F163">
+        <v>-0.48476453234550698</v>
+      </c>
+      <c r="G163">
+        <v>1</v>
+      </c>
+      <c r="H163">
+        <v>0</v>
+      </c>
+      <c r="I163" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>1</v>
+      </c>
+      <c r="B164">
+        <v>0</v>
+      </c>
+      <c r="C164">
+        <v>-0.24830091901610099</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+      <c r="E164">
+        <v>1</v>
+      </c>
+      <c r="F164">
+        <v>0.13601868824277</v>
+      </c>
+      <c r="G164">
+        <v>0</v>
+      </c>
+      <c r="H164">
+        <v>0</v>
+      </c>
+      <c r="I164" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>1</v>
+      </c>
+      <c r="B165">
+        <v>0</v>
+      </c>
+      <c r="C165">
+        <v>-0.21949345156406999</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+      <c r="E165">
+        <v>0</v>
+      </c>
+      <c r="F165">
+        <v>-0.43558635626084502</v>
+      </c>
+      <c r="G165">
+        <v>0</v>
+      </c>
+      <c r="H165">
+        <v>0</v>
+      </c>
+      <c r="I165" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>0</v>
+      </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
+      <c r="C166">
+        <v>-5.8100402117764002E-2</v>
+      </c>
+      <c r="D166">
+        <v>1</v>
+      </c>
+      <c r="E166">
+        <v>0</v>
+      </c>
+      <c r="F166">
+        <v>-0.23409079095326099</v>
+      </c>
+      <c r="G166">
+        <v>0</v>
+      </c>
+      <c r="H166">
+        <v>1</v>
+      </c>
+      <c r="I166" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>1</v>
+      </c>
+      <c r="B167">
+        <v>0</v>
+      </c>
+      <c r="C167">
+        <v>-0.14650659833260399</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+      <c r="E167">
+        <v>1</v>
+      </c>
+      <c r="F167">
+        <v>-0.102358197209554</v>
+      </c>
+      <c r="G167">
+        <v>1</v>
+      </c>
+      <c r="H167">
+        <v>0</v>
+      </c>
+      <c r="I167" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>0</v>
+      </c>
+      <c r="B168">
+        <v>0</v>
+      </c>
+      <c r="C168">
+        <v>-1.0579662439017E-2</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+      <c r="E168">
+        <v>1</v>
+      </c>
+      <c r="F168">
+        <v>5.3527157300471001E-2</v>
+      </c>
+      <c r="G168">
+        <v>1</v>
+      </c>
+      <c r="H168">
+        <v>0</v>
+      </c>
+      <c r="I168" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>1</v>
+      </c>
+      <c r="B169">
+        <v>0</v>
+      </c>
+      <c r="C169">
+        <v>-0.129669708343046</v>
+      </c>
+      <c r="D169">
+        <v>0</v>
+      </c>
+      <c r="E169">
+        <v>0</v>
+      </c>
+      <c r="F169">
+        <v>-7.6827388314038E-2</v>
+      </c>
+      <c r="G169">
+        <v>1</v>
+      </c>
+      <c r="H169">
+        <v>1</v>
+      </c>
+      <c r="I169" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>0</v>
+      </c>
+      <c r="B170">
+        <v>0</v>
+      </c>
+      <c r="C170">
+        <v>5.6803749813407002E-2</v>
+      </c>
+      <c r="D170">
+        <v>1</v>
+      </c>
+      <c r="E170">
+        <v>1</v>
+      </c>
+      <c r="F170">
+        <v>3.6414817824587997E-2</v>
+      </c>
+      <c r="G170">
+        <v>0</v>
+      </c>
+      <c r="H170">
+        <v>0</v>
+      </c>
+      <c r="I170" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>1</v>
+      </c>
+      <c r="B171">
+        <v>0</v>
+      </c>
+      <c r="C171">
+        <v>-0.24899884616986301</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171">
+        <v>0</v>
+      </c>
+      <c r="F171">
+        <v>5.3850852399185002E-2</v>
+      </c>
+      <c r="G171">
+        <v>0</v>
+      </c>
+      <c r="H171">
+        <v>1</v>
+      </c>
+      <c r="I171" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>1</v>
+      </c>
+      <c r="B172">
+        <v>0</v>
+      </c>
+      <c r="C172">
+        <v>-0.210634692293486</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+      <c r="E172">
+        <v>1</v>
+      </c>
+      <c r="F172">
+        <v>0.111898161912733</v>
+      </c>
+      <c r="G172">
+        <v>0</v>
+      </c>
+      <c r="H172">
+        <v>0</v>
+      </c>
+      <c r="I172" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>1</v>
+      </c>
+      <c r="B173">
+        <v>0</v>
+      </c>
+      <c r="C173">
+        <v>-0.15857498621185501</v>
+      </c>
+      <c r="D173">
+        <v>1</v>
+      </c>
+      <c r="E173">
+        <v>0</v>
+      </c>
+      <c r="F173">
+        <v>-0.60627519902109095</v>
+      </c>
+      <c r="G173">
+        <v>1</v>
+      </c>
+      <c r="H173">
+        <v>0</v>
+      </c>
+      <c r="I173" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>1</v>
+      </c>
+      <c r="B174">
+        <v>1</v>
+      </c>
+      <c r="C174">
+        <v>5.4692322696633003E-2</v>
+      </c>
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174">
+        <v>0</v>
+      </c>
+      <c r="F174">
+        <v>-6.5608157148340004E-3</v>
+      </c>
+      <c r="G174">
+        <v>1</v>
+      </c>
+      <c r="H174">
+        <v>0</v>
+      </c>
+      <c r="I174" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>0</v>
+      </c>
+      <c r="B175">
+        <v>0</v>
+      </c>
+      <c r="C175">
+        <v>7.7228202419988998E-2</v>
+      </c>
+      <c r="D175">
+        <v>1</v>
+      </c>
+      <c r="E175">
+        <v>1</v>
+      </c>
+      <c r="F175">
+        <v>4.3006180541197002E-2</v>
+      </c>
+      <c r="G175">
+        <v>1</v>
+      </c>
+      <c r="H175">
+        <v>0</v>
+      </c>
+      <c r="I175" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>1</v>
+      </c>
+      <c r="B176">
+        <v>0</v>
+      </c>
+      <c r="C176">
+        <v>-0.106523636781959</v>
+      </c>
+      <c r="D176">
+        <v>0</v>
+      </c>
+      <c r="E176">
+        <v>0</v>
+      </c>
+      <c r="F176">
+        <v>-5.0748104751218E-2</v>
+      </c>
+      <c r="G176">
+        <v>1</v>
+      </c>
+      <c r="H176">
+        <v>1</v>
+      </c>
+      <c r="I176" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>1</v>
+      </c>
+      <c r="B177">
+        <v>0</v>
+      </c>
+      <c r="C177">
+        <v>-0.215347846344532</v>
+      </c>
+      <c r="D177">
+        <v>0</v>
+      </c>
+      <c r="E177">
+        <v>1</v>
+      </c>
+      <c r="F177">
+        <v>0.34012677828632099</v>
+      </c>
+      <c r="G177">
+        <v>1</v>
+      </c>
+      <c r="H177">
+        <v>0</v>
+      </c>
+      <c r="I177" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>1</v>
+      </c>
+      <c r="B178">
+        <v>0</v>
+      </c>
+      <c r="C178">
+        <v>-0.26645940800590801</v>
+      </c>
+      <c r="D178">
+        <v>1</v>
+      </c>
+      <c r="E178">
+        <v>0</v>
+      </c>
+      <c r="F178">
+        <v>-0.51969756648489096</v>
+      </c>
+      <c r="G178">
+        <v>0</v>
+      </c>
+      <c r="H178">
+        <v>0</v>
+      </c>
+      <c r="I178" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>0</v>
+      </c>
+      <c r="B179">
+        <v>0</v>
+      </c>
+      <c r="C179">
+        <v>6.3949118327960006E-2</v>
+      </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
+      <c r="E179">
+        <v>1</v>
+      </c>
+      <c r="F179">
+        <v>0.29838768511636199</v>
+      </c>
+      <c r="G179">
+        <v>1</v>
+      </c>
+      <c r="H179">
+        <v>1</v>
+      </c>
+      <c r="I179" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>1</v>
+      </c>
+      <c r="B180">
+        <v>0</v>
+      </c>
+      <c r="C180">
+        <v>-0.261043410456471</v>
+      </c>
+      <c r="D180">
+        <v>0</v>
+      </c>
+      <c r="E180">
+        <v>0</v>
+      </c>
+      <c r="F180">
+        <v>5.3045221091124001E-2</v>
+      </c>
+      <c r="G180">
+        <v>0</v>
+      </c>
+      <c r="H180">
+        <v>0</v>
+      </c>
+      <c r="I180" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>0</v>
+      </c>
+      <c r="B181">
+        <v>0</v>
+      </c>
+      <c r="C181">
+        <v>4.4074604013224002E-2</v>
+      </c>
+      <c r="D181">
+        <v>1</v>
+      </c>
+      <c r="E181">
+        <v>1</v>
+      </c>
+      <c r="F181">
+        <v>0.108815578113061</v>
+      </c>
+      <c r="G181">
+        <v>0</v>
+      </c>
+      <c r="H181">
+        <v>1</v>
+      </c>
+      <c r="I181" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>1</v>
+      </c>
+      <c r="B182">
+        <v>0</v>
+      </c>
+      <c r="C182">
+        <v>-0.30095364422906001</v>
+      </c>
+      <c r="D182">
+        <v>1</v>
+      </c>
+      <c r="E182">
+        <v>0</v>
+      </c>
+      <c r="F182">
+        <v>-0.55929207108580703</v>
+      </c>
+      <c r="G182">
+        <v>0</v>
+      </c>
+      <c r="H182">
+        <v>0</v>
+      </c>
+      <c r="I182" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>1</v>
+      </c>
+      <c r="B183">
+        <v>0</v>
+      </c>
+      <c r="C183">
+        <v>-0.198394875151477</v>
+      </c>
+      <c r="D183">
+        <v>1</v>
+      </c>
+      <c r="E183">
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <v>-0.79751769340562695</v>
+      </c>
+      <c r="G183">
+        <v>0</v>
+      </c>
+      <c r="H183">
+        <v>1</v>
+      </c>
+      <c r="I183" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>1</v>
+      </c>
+      <c r="B184">
+        <v>0</v>
+      </c>
+      <c r="C184">
+        <v>-0.318575406553676</v>
+      </c>
+      <c r="D184">
+        <v>1</v>
+      </c>
+      <c r="E184">
+        <v>0</v>
+      </c>
+      <c r="F184">
+        <v>-0.55575744544887395</v>
+      </c>
+      <c r="G184">
+        <v>0</v>
+      </c>
+      <c r="H184">
+        <v>0</v>
+      </c>
+      <c r="I184" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>0</v>
+      </c>
+      <c r="B185">
+        <v>0</v>
+      </c>
+      <c r="C185">
+        <v>2.0674783175012E-2</v>
+      </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
+      <c r="E185">
+        <v>1</v>
+      </c>
+      <c r="F185">
+        <v>1.566754412008E-2</v>
+      </c>
+      <c r="G185">
+        <v>1</v>
+      </c>
+      <c r="H185">
+        <v>1</v>
+      </c>
+      <c r="I185" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>1</v>
+      </c>
+      <c r="B186">
+        <v>0</v>
+      </c>
+      <c r="C186">
+        <v>-0.118545897850774</v>
+      </c>
+      <c r="D186">
+        <v>1</v>
+      </c>
+      <c r="E186">
+        <v>0</v>
+      </c>
+      <c r="F186">
+        <v>-0.40103456746856198</v>
+      </c>
+      <c r="G186">
+        <v>1</v>
+      </c>
+      <c r="H186">
+        <v>0</v>
+      </c>
+      <c r="I186" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>0</v>
+      </c>
+      <c r="B187">
+        <v>0</v>
+      </c>
+      <c r="C187">
+        <v>-1.3854062773072001E-2</v>
+      </c>
+      <c r="D187">
+        <v>1</v>
+      </c>
+      <c r="E187">
+        <v>1</v>
+      </c>
+      <c r="F187">
+        <v>0.15449187048353499</v>
+      </c>
+      <c r="G187">
+        <v>0</v>
+      </c>
+      <c r="H187">
+        <v>1</v>
+      </c>
+      <c r="I187" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>1</v>
+      </c>
+      <c r="B188">
+        <v>0</v>
+      </c>
+      <c r="C188">
+        <v>-0.12981971808269699</v>
+      </c>
+      <c r="D188">
+        <v>1</v>
+      </c>
+      <c r="E188">
+        <v>0</v>
+      </c>
+      <c r="F188">
+        <v>-0.32223675810222702</v>
+      </c>
+      <c r="G188">
+        <v>1</v>
+      </c>
+      <c r="H188">
+        <v>0</v>
+      </c>
+      <c r="I188" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>0</v>
+      </c>
+      <c r="B189">
+        <v>0</v>
+      </c>
+      <c r="C189">
+        <v>-7.8732054803659999E-3</v>
+      </c>
+      <c r="D189">
+        <v>1</v>
+      </c>
+      <c r="E189">
+        <v>1</v>
+      </c>
+      <c r="F189">
+        <v>8.9693627769900003E-2</v>
+      </c>
+      <c r="G189">
+        <v>0</v>
+      </c>
+      <c r="H189">
+        <v>1</v>
+      </c>
+      <c r="I189" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>1</v>
+      </c>
+      <c r="B190">
+        <v>0</v>
+      </c>
+      <c r="C190">
+        <v>-0.306645991026959</v>
+      </c>
+      <c r="D190">
+        <v>0</v>
+      </c>
+      <c r="E190">
+        <v>1</v>
+      </c>
+      <c r="F190">
+        <v>0.16959247085927801</v>
+      </c>
+      <c r="G190">
+        <v>1</v>
+      </c>
+      <c r="H190">
+        <v>1</v>
+      </c>
+      <c r="I190" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>0</v>
+      </c>
+      <c r="B191">
+        <v>1</v>
+      </c>
+      <c r="C191">
+        <v>0.14673823864844401</v>
+      </c>
+      <c r="D191">
+        <v>1</v>
+      </c>
+      <c r="E191">
+        <v>0</v>
+      </c>
+      <c r="F191">
+        <v>-0.134400307118895</v>
+      </c>
+      <c r="G191">
+        <v>0</v>
+      </c>
+      <c r="H191">
+        <v>1</v>
+      </c>
+      <c r="I191" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>0</v>
+      </c>
+      <c r="B192">
+        <v>0</v>
+      </c>
+      <c r="C192">
+        <v>-4.9962808738591998E-2</v>
+      </c>
+      <c r="D192">
+        <v>0</v>
+      </c>
+      <c r="E192">
+        <v>1</v>
+      </c>
+      <c r="F192">
+        <v>0.142427662449811</v>
+      </c>
+      <c r="G192">
+        <v>1</v>
+      </c>
+      <c r="H192">
+        <v>0</v>
+      </c>
+      <c r="I192" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>0</v>
+      </c>
+      <c r="B193">
+        <v>0</v>
+      </c>
+      <c r="C193">
+        <v>-1.9671384768967001E-2</v>
+      </c>
+      <c r="D193">
+        <v>1</v>
+      </c>
+      <c r="E193">
+        <v>1</v>
+      </c>
+      <c r="F193">
+        <v>0.195014189728278</v>
+      </c>
+      <c r="G193">
+        <v>0</v>
+      </c>
+      <c r="H193">
+        <v>1</v>
+      </c>
+      <c r="I193" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>1</v>
+      </c>
+      <c r="B194">
+        <v>0</v>
+      </c>
+      <c r="C194">
+        <v>-0.54490809907292104</v>
+      </c>
+      <c r="D194">
+        <v>0</v>
+      </c>
+      <c r="E194">
+        <v>0</v>
+      </c>
+      <c r="F194">
+        <v>-0.13016973380887301</v>
+      </c>
+      <c r="G194">
+        <v>1</v>
+      </c>
+      <c r="H194">
+        <v>1</v>
+      </c>
+      <c r="I194" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>0</v>
+      </c>
+      <c r="B195">
+        <v>1</v>
+      </c>
+      <c r="C195">
+        <v>0.30598168043440999</v>
+      </c>
+      <c r="D195">
+        <v>1</v>
+      </c>
+      <c r="E195">
+        <v>1</v>
+      </c>
+      <c r="F195">
+        <v>0.12236216186283499</v>
+      </c>
+      <c r="G195">
+        <v>0</v>
+      </c>
+      <c r="H195">
+        <v>0</v>
+      </c>
+      <c r="I195" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>1</v>
+      </c>
+      <c r="B196">
+        <v>0</v>
+      </c>
+      <c r="C196">
+        <v>-0.42865035050585798</v>
+      </c>
+      <c r="D196">
+        <v>0</v>
+      </c>
+      <c r="E196">
+        <v>1</v>
+      </c>
+      <c r="F196">
+        <v>0.19445316126635501</v>
+      </c>
+      <c r="G196">
+        <v>0</v>
+      </c>
+      <c r="H196">
+        <v>1</v>
+      </c>
+      <c r="I196" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>0</v>
+      </c>
+      <c r="B197">
+        <v>0</v>
+      </c>
+      <c r="C197">
+        <v>-0.14972320697792299</v>
+      </c>
+      <c r="D197">
+        <v>1</v>
+      </c>
+      <c r="E197">
+        <v>1</v>
+      </c>
+      <c r="F197">
+        <v>8.0474869396283996E-2</v>
+      </c>
+      <c r="G197">
+        <v>0</v>
+      </c>
+      <c r="H197">
+        <v>1</v>
+      </c>
+      <c r="I197" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>1</v>
+      </c>
+      <c r="B198">
+        <v>0</v>
+      </c>
+      <c r="C198">
+        <v>-0.43946296926540801</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198">
+        <v>1</v>
+      </c>
+      <c r="F198">
+        <v>0.16134356041512099</v>
+      </c>
+      <c r="G198">
+        <v>0</v>
+      </c>
+      <c r="H198">
+        <v>1</v>
+      </c>
+      <c r="I198" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>1</v>
+      </c>
+      <c r="B199">
+        <v>0</v>
+      </c>
+      <c r="C199">
+        <v>-0.24447479789436199</v>
+      </c>
+      <c r="D199">
+        <v>0</v>
+      </c>
+      <c r="E199">
+        <v>1</v>
+      </c>
+      <c r="F199">
+        <v>0.43855083707333797</v>
+      </c>
+      <c r="G199">
+        <v>0</v>
+      </c>
+      <c r="H199">
+        <v>1</v>
+      </c>
+      <c r="I199" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>1</v>
+      </c>
+      <c r="B200">
+        <v>0</v>
+      </c>
+      <c r="C200">
+        <v>-0.50390764153702405</v>
+      </c>
+      <c r="D200">
+        <v>1</v>
+      </c>
+      <c r="E200">
+        <v>0</v>
+      </c>
+      <c r="F200">
+        <v>-0.56172970395785304</v>
+      </c>
+      <c r="G200">
+        <v>0</v>
+      </c>
+      <c r="H200">
+        <v>0</v>
+      </c>
+      <c r="I200" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>0</v>
+      </c>
+      <c r="B201">
+        <v>1</v>
+      </c>
+      <c r="C201">
+        <v>0.24985027346743</v>
+      </c>
+      <c r="D201">
+        <v>1</v>
+      </c>
+      <c r="E201">
+        <v>0</v>
+      </c>
+      <c r="F201">
+        <v>-0.208583245689962</v>
+      </c>
+      <c r="G201">
+        <v>0</v>
+      </c>
+      <c r="H201">
+        <v>1</v>
+      </c>
+      <c r="I201" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>1</v>
+      </c>
+      <c r="B202">
+        <v>0</v>
+      </c>
+      <c r="C202">
+        <v>-0.17083155567511399</v>
+      </c>
+      <c r="D202">
+        <v>0</v>
+      </c>
+      <c r="E202">
+        <v>0</v>
+      </c>
+      <c r="F202">
+        <v>-0.133666106055743</v>
+      </c>
+      <c r="G202">
+        <v>1</v>
+      </c>
+      <c r="H202">
+        <v>1</v>
+      </c>
+      <c r="I202" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>0</v>
+      </c>
+      <c r="B203">
+        <v>1</v>
+      </c>
+      <c r="C203">
+        <v>0.14683020355340501</v>
+      </c>
+      <c r="D203">
+        <v>1</v>
+      </c>
+      <c r="E203">
+        <v>0</v>
+      </c>
+      <c r="F203">
+        <v>-0.146206997284517</v>
+      </c>
+      <c r="G203">
+        <v>0</v>
+      </c>
+      <c r="H203">
+        <v>1</v>
+      </c>
+      <c r="I203" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>1</v>
+      </c>
+      <c r="B204">
+        <v>0</v>
+      </c>
+      <c r="C204">
+        <v>-0.59051694841067603</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
+      </c>
+      <c r="E204">
+        <v>0</v>
+      </c>
+      <c r="F204">
+        <v>-0.14642099695747701</v>
+      </c>
+      <c r="G204">
+        <v>1</v>
+      </c>
+      <c r="H204">
+        <v>1</v>
+      </c>
+      <c r="I204" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>0</v>
+      </c>
+      <c r="B205">
+        <v>1</v>
+      </c>
+      <c r="C205">
+        <v>0.37885891194193</v>
+      </c>
+      <c r="D205">
+        <v>1</v>
+      </c>
+      <c r="E205">
+        <v>1</v>
+      </c>
+      <c r="F205">
+        <v>6.5743605398059998E-2</v>
+      </c>
+      <c r="G205">
+        <v>1</v>
+      </c>
+      <c r="H205">
+        <v>1</v>
+      </c>
+      <c r="I205" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>1</v>
+      </c>
+      <c r="B206">
+        <v>0</v>
+      </c>
+      <c r="C206">
+        <v>-0.55458881579053299</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="E206">
+        <v>1</v>
+      </c>
+      <c r="F206">
+        <v>0.20346580355836399</v>
+      </c>
+      <c r="G206">
+        <v>0</v>
+      </c>
+      <c r="H206">
+        <v>1</v>
+      </c>
+      <c r="I206" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>0</v>
+      </c>
+      <c r="B207">
+        <v>1</v>
+      </c>
+      <c r="C207">
+        <v>0.31217564923102897</v>
+      </c>
+      <c r="D207">
+        <v>1</v>
+      </c>
+      <c r="E207">
+        <v>0</v>
+      </c>
+      <c r="F207">
+        <v>-0.32759151821203403</v>
+      </c>
+      <c r="G207">
+        <v>0</v>
+      </c>
+      <c r="H207">
+        <v>1</v>
+      </c>
+      <c r="I207" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>1</v>
+      </c>
+      <c r="B208">
+        <v>0</v>
+      </c>
+      <c r="C208">
+        <v>-0.48704773438031301</v>
+      </c>
+      <c r="D208">
+        <v>0</v>
+      </c>
+      <c r="E208">
+        <v>1</v>
+      </c>
+      <c r="F208">
+        <v>0.121166530661194</v>
+      </c>
+      <c r="G208">
+        <v>0</v>
+      </c>
+      <c r="H208">
+        <v>0</v>
+      </c>
+      <c r="I208" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>1</v>
+      </c>
+      <c r="B209">
+        <v>1</v>
+      </c>
+      <c r="C209">
+        <v>9.2275264661579991E-3</v>
+      </c>
+      <c r="D209">
+        <v>1</v>
+      </c>
+      <c r="E209">
+        <v>0</v>
+      </c>
+      <c r="F209">
+        <v>-0.18725013160795601</v>
+      </c>
+      <c r="G209">
+        <v>1</v>
+      </c>
+      <c r="H209">
+        <v>1</v>
+      </c>
+      <c r="I209" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>1</v>
+      </c>
+      <c r="B210">
+        <v>0</v>
+      </c>
+      <c r="C210">
+        <v>-0.51377167984321404</v>
+      </c>
+      <c r="D210">
+        <v>0</v>
+      </c>
+      <c r="E210">
+        <v>1</v>
+      </c>
+      <c r="F210">
+        <v>0.20801115675089099</v>
+      </c>
+      <c r="G210">
+        <v>0</v>
+      </c>
+      <c r="H210">
+        <v>1</v>
+      </c>
+      <c r="I210" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
i think ive fixed the trigger problem
</commit_message>
<xml_diff>
--- a/decision_data.xlsx
+++ b/decision_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BFE1708F-69BB-42DA-860D-63D46AB46265}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D246D432-2AA5-4A25-8268-7CEE930D713B}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26115" yWindow="2685" windowWidth="21600" windowHeight="11385" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="decision_data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="data_no_higher_order" sheetId="15" r:id="rId7"/>
     <sheet name="increased_gain" sheetId="16" r:id="rId8"/>
     <sheet name="schema_2" sheetId="17" r:id="rId9"/>
-    <sheet name="schema_1" sheetId="19" r:id="rId10"/>
+    <sheet name="scheme_1" sheetId="19" r:id="rId10"/>
     <sheet name="schema_2_continuous" sheetId="18" r:id="rId11"/>
   </sheets>
   <definedNames>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="29">
   <si>
     <t>first_peak</t>
   </si>
@@ -6567,26 +6567,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2990638-EA7F-499C-9830-7D76C07FFC26}">
-  <dimension ref="A1:K125"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A1F1DB-53E2-4230-84C6-C3B0BD8E5FC9}">
+  <dimension ref="A1:K193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K125"/>
+      <selection activeCell="A2" sqref="A2:K193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -10960,6 +10948,2386 @@
         <v>1</v>
       </c>
       <c r="K125" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>1</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="C126">
+        <v>0.12587834759376601</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+      <c r="E126">
+        <v>1</v>
+      </c>
+      <c r="F126">
+        <v>3.4911583468922001E-2</v>
+      </c>
+      <c r="G126">
+        <v>0</v>
+      </c>
+      <c r="H126">
+        <v>1</v>
+      </c>
+      <c r="I126">
+        <v>1</v>
+      </c>
+      <c r="J126">
+        <v>1</v>
+      </c>
+      <c r="K126" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>0</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127">
+        <v>-6.9586179404461004E-2</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127">
+        <v>1</v>
+      </c>
+      <c r="F127">
+        <v>3.1252497288195E-2</v>
+      </c>
+      <c r="G127">
+        <v>1</v>
+      </c>
+      <c r="H127">
+        <v>0</v>
+      </c>
+      <c r="I127">
+        <v>0</v>
+      </c>
+      <c r="J127">
+        <v>0</v>
+      </c>
+      <c r="K127" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>1</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>9.8359058045160999E-2</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>1</v>
+      </c>
+      <c r="F128">
+        <v>3.8313836869165001E-2</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+      <c r="H128">
+        <v>1</v>
+      </c>
+      <c r="I128">
+        <v>1</v>
+      </c>
+      <c r="J128">
+        <v>1</v>
+      </c>
+      <c r="K128" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>1</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+      <c r="C129">
+        <v>0.135312389836899</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+      <c r="F129">
+        <v>0.12216818475437401</v>
+      </c>
+      <c r="G129">
+        <v>0</v>
+      </c>
+      <c r="H129">
+        <v>0</v>
+      </c>
+      <c r="I129">
+        <v>1</v>
+      </c>
+      <c r="J129">
+        <v>1</v>
+      </c>
+      <c r="K129" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>0</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130">
+        <v>-2.9746967690679998E-2</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <v>4.7307840966217998E-2</v>
+      </c>
+      <c r="G130">
+        <v>1</v>
+      </c>
+      <c r="H130">
+        <v>1</v>
+      </c>
+      <c r="I130">
+        <v>0</v>
+      </c>
+      <c r="J130">
+        <v>1</v>
+      </c>
+      <c r="K130" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>1</v>
+      </c>
+      <c r="B131">
+        <v>0</v>
+      </c>
+      <c r="C131">
+        <v>6.7311247749722997E-2</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <v>3.1412841990926997E-2</v>
+      </c>
+      <c r="G131">
+        <v>0</v>
+      </c>
+      <c r="H131">
+        <v>0</v>
+      </c>
+      <c r="I131">
+        <v>1</v>
+      </c>
+      <c r="J131">
+        <v>1</v>
+      </c>
+      <c r="K131" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>0</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+      <c r="C132">
+        <v>-5.0151019876452999E-2</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="F132">
+        <v>0.12721529553908301</v>
+      </c>
+      <c r="G132">
+        <v>1</v>
+      </c>
+      <c r="H132">
+        <v>0</v>
+      </c>
+      <c r="I132">
+        <v>0</v>
+      </c>
+      <c r="J132">
+        <v>1</v>
+      </c>
+      <c r="K132" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>1</v>
+      </c>
+      <c r="B133">
+        <v>0</v>
+      </c>
+      <c r="C133">
+        <v>3.8544184430813998E-2</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+      <c r="E133">
+        <v>1</v>
+      </c>
+      <c r="F133">
+        <v>-7.400012888535E-3</v>
+      </c>
+      <c r="G133">
+        <v>0</v>
+      </c>
+      <c r="H133">
+        <v>0</v>
+      </c>
+      <c r="I133">
+        <v>1</v>
+      </c>
+      <c r="J133">
+        <v>0</v>
+      </c>
+      <c r="K133" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>0</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134">
+        <v>-1.8566986626454E-2</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="F134">
+        <v>3.0652324702874999E-2</v>
+      </c>
+      <c r="G134">
+        <v>1</v>
+      </c>
+      <c r="H134">
+        <v>0</v>
+      </c>
+      <c r="I134">
+        <v>0</v>
+      </c>
+      <c r="J134">
+        <v>1</v>
+      </c>
+      <c r="K134" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>1</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+      <c r="C135">
+        <v>6.7482282286725995E-2</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+      <c r="E135">
+        <v>1</v>
+      </c>
+      <c r="F135">
+        <v>9.7814604588412998E-2</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
+      <c r="H135">
+        <v>0</v>
+      </c>
+      <c r="I135">
+        <v>1</v>
+      </c>
+      <c r="J135">
+        <v>1</v>
+      </c>
+      <c r="K135" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>0</v>
+      </c>
+      <c r="B136">
+        <v>1</v>
+      </c>
+      <c r="C136">
+        <v>-7.0263159185719001E-2</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+      <c r="F136">
+        <v>0.18229620410880601</v>
+      </c>
+      <c r="G136">
+        <v>1</v>
+      </c>
+      <c r="H136">
+        <v>0</v>
+      </c>
+      <c r="I136">
+        <v>0</v>
+      </c>
+      <c r="J136">
+        <v>1</v>
+      </c>
+      <c r="K136" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>0</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+      <c r="C137">
+        <v>-1.7671020448010999E-2</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+      <c r="E137">
+        <v>1</v>
+      </c>
+      <c r="F137">
+        <v>0.114249096546259</v>
+      </c>
+      <c r="G137">
+        <v>1</v>
+      </c>
+      <c r="H137">
+        <v>0</v>
+      </c>
+      <c r="I137">
+        <v>1</v>
+      </c>
+      <c r="J137">
+        <v>1</v>
+      </c>
+      <c r="K137" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>1</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+      <c r="C138">
+        <v>-1.2199308180773E-2</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+      <c r="F138">
+        <v>0.24921467510915901</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
+      <c r="H138">
+        <v>0</v>
+      </c>
+      <c r="I138">
+        <v>0</v>
+      </c>
+      <c r="J138">
+        <v>1</v>
+      </c>
+      <c r="K138" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>0</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+      <c r="C139">
+        <v>8.0092594456600003E-4</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+      <c r="E139">
+        <v>1</v>
+      </c>
+      <c r="F139">
+        <v>0.12930787271059699</v>
+      </c>
+      <c r="G139">
+        <v>1</v>
+      </c>
+      <c r="H139">
+        <v>0</v>
+      </c>
+      <c r="I139">
+        <v>1</v>
+      </c>
+      <c r="J139">
+        <v>1</v>
+      </c>
+      <c r="K139" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>1</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+      <c r="C140">
+        <v>0.13050344501354799</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+      <c r="H140">
+        <v>0</v>
+      </c>
+      <c r="I140">
+        <v>1</v>
+      </c>
+      <c r="J140">
+        <v>0</v>
+      </c>
+      <c r="K140" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>0</v>
+      </c>
+      <c r="B141">
+        <v>0</v>
+      </c>
+      <c r="C141">
+        <v>-0.121475329345405</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="E141">
+        <v>1</v>
+      </c>
+      <c r="F141">
+        <v>7.5442564160345005E-2</v>
+      </c>
+      <c r="G141">
+        <v>1</v>
+      </c>
+      <c r="H141">
+        <v>0</v>
+      </c>
+      <c r="I141">
+        <v>1</v>
+      </c>
+      <c r="J141">
+        <v>0</v>
+      </c>
+      <c r="K141" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>1</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+      <c r="C142">
+        <v>5.4331416151837002E-2</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142">
+        <v>8.8464491054556005E-2</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+      <c r="H142">
+        <v>0</v>
+      </c>
+      <c r="I142">
+        <v>1</v>
+      </c>
+      <c r="J142">
+        <v>1</v>
+      </c>
+      <c r="K142" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>1</v>
+      </c>
+      <c r="B143">
+        <v>1</v>
+      </c>
+      <c r="C143">
+        <v>2.4574020263507999E-2</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <v>2.8445782139730001E-2</v>
+      </c>
+      <c r="G143">
+        <v>0</v>
+      </c>
+      <c r="H143">
+        <v>1</v>
+      </c>
+      <c r="I143">
+        <v>0</v>
+      </c>
+      <c r="J143">
+        <v>1</v>
+      </c>
+      <c r="K143" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>1</v>
+      </c>
+      <c r="B144">
+        <v>0</v>
+      </c>
+      <c r="C144">
+        <v>6.7331902495410004E-2</v>
+      </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144">
+        <v>2.3649724651075E-2</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+      <c r="H144">
+        <v>1</v>
+      </c>
+      <c r="I144">
+        <v>1</v>
+      </c>
+      <c r="J144">
+        <v>1</v>
+      </c>
+      <c r="K144" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>0</v>
+      </c>
+      <c r="B145">
+        <v>0</v>
+      </c>
+      <c r="C145">
+        <v>5.1507649474601E-2</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145">
+        <v>0.122187262321728</v>
+      </c>
+      <c r="G145">
+        <v>1</v>
+      </c>
+      <c r="H145">
+        <v>0</v>
+      </c>
+      <c r="I145">
+        <v>1</v>
+      </c>
+      <c r="J145">
+        <v>1</v>
+      </c>
+      <c r="K145" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>1</v>
+      </c>
+      <c r="B146">
+        <v>0</v>
+      </c>
+      <c r="C146">
+        <v>0.12855152222590399</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
+      <c r="F146">
+        <v>1.6747646704168E-2</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+      <c r="H146">
+        <v>1</v>
+      </c>
+      <c r="I146">
+        <v>1</v>
+      </c>
+      <c r="J146">
+        <v>0</v>
+      </c>
+      <c r="K146" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>0</v>
+      </c>
+      <c r="B147">
+        <v>1</v>
+      </c>
+      <c r="C147">
+        <v>-0.107968465455927</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+      <c r="E147">
+        <v>1</v>
+      </c>
+      <c r="F147">
+        <v>0.20004366522040601</v>
+      </c>
+      <c r="G147">
+        <v>1</v>
+      </c>
+      <c r="H147">
+        <v>0</v>
+      </c>
+      <c r="I147">
+        <v>0</v>
+      </c>
+      <c r="J147">
+        <v>0</v>
+      </c>
+      <c r="K147" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>1</v>
+      </c>
+      <c r="B148">
+        <v>0</v>
+      </c>
+      <c r="C148">
+        <v>0.11977190361734701</v>
+      </c>
+      <c r="D148">
+        <v>0</v>
+      </c>
+      <c r="E148">
+        <v>1</v>
+      </c>
+      <c r="F148">
+        <v>0.174196811839053</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+      <c r="H148">
+        <v>1</v>
+      </c>
+      <c r="I148">
+        <v>1</v>
+      </c>
+      <c r="J148">
+        <v>1</v>
+      </c>
+      <c r="K148" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>1</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+      <c r="C149">
+        <v>2.208570158259E-2</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+      <c r="F149">
+        <v>0.16656473244874301</v>
+      </c>
+      <c r="G149">
+        <v>0</v>
+      </c>
+      <c r="H149">
+        <v>0</v>
+      </c>
+      <c r="I149">
+        <v>0</v>
+      </c>
+      <c r="J149">
+        <v>0</v>
+      </c>
+      <c r="K149" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>1</v>
+      </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
+      <c r="C150">
+        <v>0.11028810954889599</v>
+      </c>
+      <c r="D150">
+        <v>0</v>
+      </c>
+      <c r="E150">
+        <v>1</v>
+      </c>
+      <c r="F150">
+        <v>-7.2131916444890002E-3</v>
+      </c>
+      <c r="G150">
+        <v>0</v>
+      </c>
+      <c r="H150">
+        <v>1</v>
+      </c>
+      <c r="I150">
+        <v>1</v>
+      </c>
+      <c r="J150">
+        <v>0</v>
+      </c>
+      <c r="K150" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>1</v>
+      </c>
+      <c r="B151">
+        <v>0</v>
+      </c>
+      <c r="C151">
+        <v>0.164538788313775</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="F151">
+        <v>0.19769080677557099</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
+      <c r="H151">
+        <v>0</v>
+      </c>
+      <c r="I151">
+        <v>1</v>
+      </c>
+      <c r="J151">
+        <v>0</v>
+      </c>
+      <c r="K151" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>1</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <v>0.115841111204882</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <v>6.9944879180004998E-2</v>
+      </c>
+      <c r="G152">
+        <v>0</v>
+      </c>
+      <c r="H152">
+        <v>1</v>
+      </c>
+      <c r="I152">
+        <v>1</v>
+      </c>
+      <c r="J152">
+        <v>1</v>
+      </c>
+      <c r="K152" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>1</v>
+      </c>
+      <c r="B153">
+        <v>0</v>
+      </c>
+      <c r="C153">
+        <v>0.11222852490518501</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="F153">
+        <v>0.258790586906259</v>
+      </c>
+      <c r="G153">
+        <v>0</v>
+      </c>
+      <c r="H153">
+        <v>0</v>
+      </c>
+      <c r="I153">
+        <v>1</v>
+      </c>
+      <c r="J153">
+        <v>1</v>
+      </c>
+      <c r="K153" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>1</v>
+      </c>
+      <c r="B154">
+        <v>0</v>
+      </c>
+      <c r="C154">
+        <v>0.107943409499644</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
+      <c r="F154">
+        <v>0.147598323041503</v>
+      </c>
+      <c r="G154">
+        <v>0</v>
+      </c>
+      <c r="H154">
+        <v>1</v>
+      </c>
+      <c r="I154">
+        <v>1</v>
+      </c>
+      <c r="J154">
+        <v>1</v>
+      </c>
+      <c r="K154" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>1</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+      <c r="C155">
+        <v>-1.1428731271656001E-2</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+      <c r="F155">
+        <v>0.17832048849745899</v>
+      </c>
+      <c r="G155">
+        <v>0</v>
+      </c>
+      <c r="H155">
+        <v>0</v>
+      </c>
+      <c r="I155">
+        <v>0</v>
+      </c>
+      <c r="J155">
+        <v>0</v>
+      </c>
+      <c r="K155" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>1</v>
+      </c>
+      <c r="B156">
+        <v>0</v>
+      </c>
+      <c r="C156">
+        <v>0.12510275481264899</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+      <c r="F156">
+        <v>0.100298431429984</v>
+      </c>
+      <c r="G156">
+        <v>0</v>
+      </c>
+      <c r="H156">
+        <v>1</v>
+      </c>
+      <c r="I156">
+        <v>1</v>
+      </c>
+      <c r="J156">
+        <v>1</v>
+      </c>
+      <c r="K156" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>0</v>
+      </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
+      <c r="C157">
+        <v>-0.122757792618454</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+      <c r="E157">
+        <v>1</v>
+      </c>
+      <c r="F157">
+        <v>0.278534734759467</v>
+      </c>
+      <c r="G157">
+        <v>1</v>
+      </c>
+      <c r="H157">
+        <v>0</v>
+      </c>
+      <c r="I157">
+        <v>0</v>
+      </c>
+      <c r="J157">
+        <v>0</v>
+      </c>
+      <c r="K157" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>1</v>
+      </c>
+      <c r="B158">
+        <v>0</v>
+      </c>
+      <c r="C158">
+        <v>6.0936821683702999E-2</v>
+      </c>
+      <c r="D158">
+        <v>0</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="F158">
+        <v>3.5170315063290998E-2</v>
+      </c>
+      <c r="G158">
+        <v>0</v>
+      </c>
+      <c r="H158">
+        <v>1</v>
+      </c>
+      <c r="I158">
+        <v>1</v>
+      </c>
+      <c r="J158">
+        <v>1</v>
+      </c>
+      <c r="K158" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>0</v>
+      </c>
+      <c r="B159">
+        <v>0</v>
+      </c>
+      <c r="C159">
+        <v>-1.3278989861306E-2</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+      <c r="E159">
+        <v>1</v>
+      </c>
+      <c r="F159">
+        <v>0.24454415099542001</v>
+      </c>
+      <c r="G159">
+        <v>1</v>
+      </c>
+      <c r="H159">
+        <v>0</v>
+      </c>
+      <c r="I159">
+        <v>1</v>
+      </c>
+      <c r="J159">
+        <v>0</v>
+      </c>
+      <c r="K159" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>1</v>
+      </c>
+      <c r="B160">
+        <v>0</v>
+      </c>
+      <c r="C160">
+        <v>0.145737962503005</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+      <c r="F160">
+        <v>0.21381291530174201</v>
+      </c>
+      <c r="G160">
+        <v>0</v>
+      </c>
+      <c r="H160">
+        <v>0</v>
+      </c>
+      <c r="I160">
+        <v>1</v>
+      </c>
+      <c r="J160">
+        <v>1</v>
+      </c>
+      <c r="K160" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>1</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>-3.2360009542414997E-2</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+      <c r="E161">
+        <v>1</v>
+      </c>
+      <c r="F161">
+        <v>0.49155965593252399</v>
+      </c>
+      <c r="G161">
+        <v>0</v>
+      </c>
+      <c r="H161">
+        <v>0</v>
+      </c>
+      <c r="I161">
+        <v>1</v>
+      </c>
+      <c r="J161">
+        <v>1</v>
+      </c>
+      <c r="K161" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>1</v>
+      </c>
+      <c r="B162">
+        <v>0</v>
+      </c>
+      <c r="C162">
+        <v>0.10325941614380001</v>
+      </c>
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162">
+        <v>0</v>
+      </c>
+      <c r="F162">
+        <v>1.6386628311120002E-2</v>
+      </c>
+      <c r="G162">
+        <v>0</v>
+      </c>
+      <c r="H162">
+        <v>1</v>
+      </c>
+      <c r="I162">
+        <v>1</v>
+      </c>
+      <c r="J162">
+        <v>1</v>
+      </c>
+      <c r="K162" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>0</v>
+      </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
+      <c r="C163">
+        <v>-0.14264009103695199</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+      <c r="E163">
+        <v>1</v>
+      </c>
+      <c r="F163">
+        <v>0.245771390082722</v>
+      </c>
+      <c r="G163">
+        <v>1</v>
+      </c>
+      <c r="H163">
+        <v>0</v>
+      </c>
+      <c r="I163">
+        <v>0</v>
+      </c>
+      <c r="J163">
+        <v>0</v>
+      </c>
+      <c r="K163" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>1</v>
+      </c>
+      <c r="B164">
+        <v>0</v>
+      </c>
+      <c r="C164">
+        <v>0.13021483995969399</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+      <c r="E164">
+        <v>1</v>
+      </c>
+      <c r="F164">
+        <v>0.15261205967334801</v>
+      </c>
+      <c r="G164">
+        <v>0</v>
+      </c>
+      <c r="H164">
+        <v>0</v>
+      </c>
+      <c r="I164">
+        <v>1</v>
+      </c>
+      <c r="J164">
+        <v>1</v>
+      </c>
+      <c r="K164" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>0</v>
+      </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
+      <c r="C165">
+        <v>-0.18167735433553001</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+      <c r="E165">
+        <v>1</v>
+      </c>
+      <c r="F165">
+        <v>0.42678053946862499</v>
+      </c>
+      <c r="G165">
+        <v>1</v>
+      </c>
+      <c r="H165">
+        <v>0</v>
+      </c>
+      <c r="I165">
+        <v>0</v>
+      </c>
+      <c r="J165">
+        <v>1</v>
+      </c>
+      <c r="K165" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>1</v>
+      </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
+      <c r="C166">
+        <v>0.115664688674583</v>
+      </c>
+      <c r="D166">
+        <v>1</v>
+      </c>
+      <c r="E166">
+        <v>0</v>
+      </c>
+      <c r="F166">
+        <v>0.16192762659069099</v>
+      </c>
+      <c r="G166">
+        <v>0</v>
+      </c>
+      <c r="H166">
+        <v>0</v>
+      </c>
+      <c r="I166">
+        <v>1</v>
+      </c>
+      <c r="J166">
+        <v>1</v>
+      </c>
+      <c r="K166" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>1</v>
+      </c>
+      <c r="B167">
+        <v>1</v>
+      </c>
+      <c r="C167">
+        <v>-6.5771644495389997E-3</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+      <c r="E167">
+        <v>1</v>
+      </c>
+      <c r="F167">
+        <v>0.27189608971817902</v>
+      </c>
+      <c r="G167">
+        <v>0</v>
+      </c>
+      <c r="H167">
+        <v>0</v>
+      </c>
+      <c r="I167">
+        <v>0</v>
+      </c>
+      <c r="J167">
+        <v>1</v>
+      </c>
+      <c r="K167" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>1</v>
+      </c>
+      <c r="B168">
+        <v>0</v>
+      </c>
+      <c r="C168">
+        <v>0.16346250043891999</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+      <c r="E168">
+        <v>1</v>
+      </c>
+      <c r="F168">
+        <v>0.16008220286330299</v>
+      </c>
+      <c r="G168">
+        <v>0</v>
+      </c>
+      <c r="H168">
+        <v>0</v>
+      </c>
+      <c r="I168">
+        <v>1</v>
+      </c>
+      <c r="J168">
+        <v>1</v>
+      </c>
+      <c r="K168" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>1</v>
+      </c>
+      <c r="B169">
+        <v>0</v>
+      </c>
+      <c r="C169">
+        <v>9.9075773954960006E-2</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+      <c r="E169">
+        <v>1</v>
+      </c>
+      <c r="F169">
+        <v>1.4963641870507E-2</v>
+      </c>
+      <c r="G169">
+        <v>0</v>
+      </c>
+      <c r="H169">
+        <v>0</v>
+      </c>
+      <c r="I169">
+        <v>1</v>
+      </c>
+      <c r="J169">
+        <v>0</v>
+      </c>
+      <c r="K169" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>0</v>
+      </c>
+      <c r="B170">
+        <v>1</v>
+      </c>
+      <c r="C170">
+        <v>-4.9000556221567002E-2</v>
+      </c>
+      <c r="D170">
+        <v>1</v>
+      </c>
+      <c r="E170">
+        <v>1</v>
+      </c>
+      <c r="F170">
+        <v>6.2209633171937999E-2</v>
+      </c>
+      <c r="G170">
+        <v>1</v>
+      </c>
+      <c r="H170">
+        <v>0</v>
+      </c>
+      <c r="I170">
+        <v>0</v>
+      </c>
+      <c r="J170">
+        <v>0</v>
+      </c>
+      <c r="K170" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>1</v>
+      </c>
+      <c r="B171">
+        <v>0</v>
+      </c>
+      <c r="C171">
+        <v>0.102057254290186</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171">
+        <v>1</v>
+      </c>
+      <c r="F171">
+        <v>2.0021098484447001E-2</v>
+      </c>
+      <c r="G171">
+        <v>0</v>
+      </c>
+      <c r="H171">
+        <v>1</v>
+      </c>
+      <c r="I171">
+        <v>1</v>
+      </c>
+      <c r="J171">
+        <v>1</v>
+      </c>
+      <c r="K171" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>0</v>
+      </c>
+      <c r="B172">
+        <v>1</v>
+      </c>
+      <c r="C172">
+        <v>-7.1380801464027005E-2</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+      <c r="E172">
+        <v>1</v>
+      </c>
+      <c r="F172">
+        <v>3.2219859614870998E-2</v>
+      </c>
+      <c r="G172">
+        <v>1</v>
+      </c>
+      <c r="H172">
+        <v>0</v>
+      </c>
+      <c r="I172">
+        <v>0</v>
+      </c>
+      <c r="J172">
+        <v>0</v>
+      </c>
+      <c r="K172" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>1</v>
+      </c>
+      <c r="B173">
+        <v>0</v>
+      </c>
+      <c r="C173">
+        <v>5.3751833559836003E-2</v>
+      </c>
+      <c r="D173">
+        <v>1</v>
+      </c>
+      <c r="E173">
+        <v>1</v>
+      </c>
+      <c r="F173">
+        <v>-1.6025162267238002E-2</v>
+      </c>
+      <c r="G173">
+        <v>0</v>
+      </c>
+      <c r="H173">
+        <v>0</v>
+      </c>
+      <c r="I173">
+        <v>1</v>
+      </c>
+      <c r="J173">
+        <v>0</v>
+      </c>
+      <c r="K173" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>0</v>
+      </c>
+      <c r="B174">
+        <v>1</v>
+      </c>
+      <c r="C174">
+        <v>-6.2642348962186997E-2</v>
+      </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
+      <c r="E174">
+        <v>0</v>
+      </c>
+      <c r="F174">
+        <v>8.5448174226623E-2</v>
+      </c>
+      <c r="G174">
+        <v>1</v>
+      </c>
+      <c r="H174">
+        <v>0</v>
+      </c>
+      <c r="I174">
+        <v>0</v>
+      </c>
+      <c r="J174">
+        <v>1</v>
+      </c>
+      <c r="K174" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>1</v>
+      </c>
+      <c r="B175">
+        <v>0</v>
+      </c>
+      <c r="C175">
+        <v>8.5067604183791001E-2</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175">
+        <v>1</v>
+      </c>
+      <c r="F175">
+        <v>-2.6146569607001E-2</v>
+      </c>
+      <c r="G175">
+        <v>0</v>
+      </c>
+      <c r="H175">
+        <v>1</v>
+      </c>
+      <c r="I175">
+        <v>1</v>
+      </c>
+      <c r="J175">
+        <v>0</v>
+      </c>
+      <c r="K175" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>0</v>
+      </c>
+      <c r="B176">
+        <v>1</v>
+      </c>
+      <c r="C176">
+        <v>-4.1026934093399997E-2</v>
+      </c>
+      <c r="D176">
+        <v>1</v>
+      </c>
+      <c r="E176">
+        <v>1</v>
+      </c>
+      <c r="F176">
+        <v>0.257558816919154</v>
+      </c>
+      <c r="G176">
+        <v>1</v>
+      </c>
+      <c r="H176">
+        <v>0</v>
+      </c>
+      <c r="I176">
+        <v>0</v>
+      </c>
+      <c r="J176">
+        <v>1</v>
+      </c>
+      <c r="K176" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>1</v>
+      </c>
+      <c r="B177">
+        <v>0</v>
+      </c>
+      <c r="C177">
+        <v>3.7423699240194001E-2</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="E177">
+        <v>1</v>
+      </c>
+      <c r="F177">
+        <v>5.7804717541829996E-3</v>
+      </c>
+      <c r="G177">
+        <v>0</v>
+      </c>
+      <c r="H177">
+        <v>0</v>
+      </c>
+      <c r="I177">
+        <v>1</v>
+      </c>
+      <c r="J177">
+        <v>0</v>
+      </c>
+      <c r="K177" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>0</v>
+      </c>
+      <c r="B178">
+        <v>1</v>
+      </c>
+      <c r="C178">
+        <v>-6.1874523818413997E-2</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178">
+        <v>1</v>
+      </c>
+      <c r="F178">
+        <v>-1.727017648673E-3</v>
+      </c>
+      <c r="G178">
+        <v>1</v>
+      </c>
+      <c r="H178">
+        <v>1</v>
+      </c>
+      <c r="I178">
+        <v>0</v>
+      </c>
+      <c r="J178">
+        <v>0</v>
+      </c>
+      <c r="K178" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>1</v>
+      </c>
+      <c r="B179">
+        <v>1</v>
+      </c>
+      <c r="C179">
+        <v>0.121334620593191</v>
+      </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
+      <c r="E179">
+        <v>1</v>
+      </c>
+      <c r="F179">
+        <v>-1.8433882879413999E-2</v>
+      </c>
+      <c r="G179">
+        <v>0</v>
+      </c>
+      <c r="H179">
+        <v>0</v>
+      </c>
+      <c r="I179">
+        <v>0</v>
+      </c>
+      <c r="J179">
+        <v>0</v>
+      </c>
+      <c r="K179" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>1</v>
+      </c>
+      <c r="B180">
+        <v>0</v>
+      </c>
+      <c r="C180">
+        <v>9.6680478559113006E-2</v>
+      </c>
+      <c r="D180">
+        <v>0</v>
+      </c>
+      <c r="E180">
+        <v>1</v>
+      </c>
+      <c r="F180">
+        <v>8.3571593391845E-2</v>
+      </c>
+      <c r="G180">
+        <v>0</v>
+      </c>
+      <c r="H180">
+        <v>1</v>
+      </c>
+      <c r="I180">
+        <v>1</v>
+      </c>
+      <c r="J180">
+        <v>1</v>
+      </c>
+      <c r="K180" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>1</v>
+      </c>
+      <c r="B181">
+        <v>0</v>
+      </c>
+      <c r="C181">
+        <v>8.3485766432251002E-2</v>
+      </c>
+      <c r="D181">
+        <v>1</v>
+      </c>
+      <c r="E181">
+        <v>1</v>
+      </c>
+      <c r="F181">
+        <v>-2.4235489941359998E-3</v>
+      </c>
+      <c r="G181">
+        <v>0</v>
+      </c>
+      <c r="H181">
+        <v>0</v>
+      </c>
+      <c r="I181">
+        <v>1</v>
+      </c>
+      <c r="J181">
+        <v>0</v>
+      </c>
+      <c r="K181" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>0</v>
+      </c>
+      <c r="B182">
+        <v>0</v>
+      </c>
+      <c r="C182">
+        <v>-3.5033668162458002E-2</v>
+      </c>
+      <c r="D182">
+        <v>1</v>
+      </c>
+      <c r="E182">
+        <v>0</v>
+      </c>
+      <c r="F182">
+        <v>9.0226586238517995E-2</v>
+      </c>
+      <c r="G182">
+        <v>1</v>
+      </c>
+      <c r="H182">
+        <v>0</v>
+      </c>
+      <c r="I182">
+        <v>1</v>
+      </c>
+      <c r="J182">
+        <v>1</v>
+      </c>
+      <c r="K182" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>1</v>
+      </c>
+      <c r="B183">
+        <v>0</v>
+      </c>
+      <c r="C183">
+        <v>9.8813416764808995E-2</v>
+      </c>
+      <c r="D183">
+        <v>1</v>
+      </c>
+      <c r="E183">
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <v>7.2200216511165996E-2</v>
+      </c>
+      <c r="G183">
+        <v>0</v>
+      </c>
+      <c r="H183">
+        <v>0</v>
+      </c>
+      <c r="I183">
+        <v>1</v>
+      </c>
+      <c r="J183">
+        <v>1</v>
+      </c>
+      <c r="K183" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>0</v>
+      </c>
+      <c r="B184">
+        <v>0</v>
+      </c>
+      <c r="C184">
+        <v>3.6429096606767998E-2</v>
+      </c>
+      <c r="D184">
+        <v>1</v>
+      </c>
+      <c r="E184">
+        <v>1</v>
+      </c>
+      <c r="F184">
+        <v>2.2699645821509999E-3</v>
+      </c>
+      <c r="G184">
+        <v>1</v>
+      </c>
+      <c r="H184">
+        <v>0</v>
+      </c>
+      <c r="I184">
+        <v>1</v>
+      </c>
+      <c r="J184">
+        <v>0</v>
+      </c>
+      <c r="K184" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>1</v>
+      </c>
+      <c r="B185">
+        <v>1</v>
+      </c>
+      <c r="C185">
+        <v>7.0115361094648998E-2</v>
+      </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
+      <c r="E185">
+        <v>1</v>
+      </c>
+      <c r="F185">
+        <v>4.4310171888179997E-2</v>
+      </c>
+      <c r="G185">
+        <v>0</v>
+      </c>
+      <c r="H185">
+        <v>0</v>
+      </c>
+      <c r="I185">
+        <v>0</v>
+      </c>
+      <c r="J185">
+        <v>0</v>
+      </c>
+      <c r="K185" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>1</v>
+      </c>
+      <c r="B186">
+        <v>0</v>
+      </c>
+      <c r="C186">
+        <v>4.3129725917827003E-2</v>
+      </c>
+      <c r="D186">
+        <v>1</v>
+      </c>
+      <c r="E186">
+        <v>1</v>
+      </c>
+      <c r="F186">
+        <v>5.7085456422907001E-2</v>
+      </c>
+      <c r="G186">
+        <v>0</v>
+      </c>
+      <c r="H186">
+        <v>0</v>
+      </c>
+      <c r="I186">
+        <v>1</v>
+      </c>
+      <c r="J186">
+        <v>1</v>
+      </c>
+      <c r="K186" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>0</v>
+      </c>
+      <c r="B187">
+        <v>1</v>
+      </c>
+      <c r="C187">
+        <v>-3.3297925541104001E-2</v>
+      </c>
+      <c r="D187">
+        <v>1</v>
+      </c>
+      <c r="E187">
+        <v>1</v>
+      </c>
+      <c r="F187">
+        <v>7.8133431767489995E-3</v>
+      </c>
+      <c r="G187">
+        <v>1</v>
+      </c>
+      <c r="H187">
+        <v>0</v>
+      </c>
+      <c r="I187">
+        <v>0</v>
+      </c>
+      <c r="J187">
+        <v>0</v>
+      </c>
+      <c r="K187" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>1</v>
+      </c>
+      <c r="B188">
+        <v>0</v>
+      </c>
+      <c r="C188">
+        <v>0.106358299154435</v>
+      </c>
+      <c r="D188">
+        <v>0</v>
+      </c>
+      <c r="E188">
+        <v>1</v>
+      </c>
+      <c r="F188">
+        <v>-5.3710240442535001E-2</v>
+      </c>
+      <c r="G188">
+        <v>0</v>
+      </c>
+      <c r="H188">
+        <v>1</v>
+      </c>
+      <c r="I188">
+        <v>1</v>
+      </c>
+      <c r="J188">
+        <v>0</v>
+      </c>
+      <c r="K188" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>0</v>
+      </c>
+      <c r="B189">
+        <v>0</v>
+      </c>
+      <c r="C189">
+        <v>-3.1682587699729002E-2</v>
+      </c>
+      <c r="D189">
+        <v>1</v>
+      </c>
+      <c r="E189">
+        <v>1</v>
+      </c>
+      <c r="F189">
+        <v>6.7197061656886006E-2</v>
+      </c>
+      <c r="G189">
+        <v>1</v>
+      </c>
+      <c r="H189">
+        <v>0</v>
+      </c>
+      <c r="I189">
+        <v>1</v>
+      </c>
+      <c r="J189">
+        <v>0</v>
+      </c>
+      <c r="K189" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>1</v>
+      </c>
+      <c r="B190">
+        <v>0</v>
+      </c>
+      <c r="C190">
+        <v>7.2168419648430002E-2</v>
+      </c>
+      <c r="D190">
+        <v>1</v>
+      </c>
+      <c r="E190">
+        <v>0</v>
+      </c>
+      <c r="F190">
+        <v>6.7835195800275999E-2</v>
+      </c>
+      <c r="G190">
+        <v>0</v>
+      </c>
+      <c r="H190">
+        <v>0</v>
+      </c>
+      <c r="I190">
+        <v>1</v>
+      </c>
+      <c r="J190">
+        <v>1</v>
+      </c>
+      <c r="K190" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>1</v>
+      </c>
+      <c r="B191">
+        <v>1</v>
+      </c>
+      <c r="C191">
+        <v>-2.023650852169E-3</v>
+      </c>
+      <c r="D191">
+        <v>1</v>
+      </c>
+      <c r="E191">
+        <v>1</v>
+      </c>
+      <c r="F191">
+        <v>0.17615785772753201</v>
+      </c>
+      <c r="G191">
+        <v>0</v>
+      </c>
+      <c r="H191">
+        <v>0</v>
+      </c>
+      <c r="I191">
+        <v>0</v>
+      </c>
+      <c r="J191">
+        <v>1</v>
+      </c>
+      <c r="K191" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>1</v>
+      </c>
+      <c r="B192">
+        <v>0</v>
+      </c>
+      <c r="C192">
+        <v>-5.7332836462008999E-2</v>
+      </c>
+      <c r="D192">
+        <v>0</v>
+      </c>
+      <c r="E192">
+        <v>0</v>
+      </c>
+      <c r="F192">
+        <v>0.31792420655674303</v>
+      </c>
+      <c r="G192">
+        <v>0</v>
+      </c>
+      <c r="H192">
+        <v>1</v>
+      </c>
+      <c r="I192">
+        <v>1</v>
+      </c>
+      <c r="J192">
+        <v>1</v>
+      </c>
+      <c r="K192" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>1</v>
+      </c>
+      <c r="B193">
+        <v>1</v>
+      </c>
+      <c r="C193">
+        <v>4.9444954157733E-2</v>
+      </c>
+      <c r="D193">
+        <v>1</v>
+      </c>
+      <c r="E193">
+        <v>0</v>
+      </c>
+      <c r="F193">
+        <v>8.6611415019430996E-2</v>
+      </c>
+      <c r="G193">
+        <v>0</v>
+      </c>
+      <c r="H193">
+        <v>0</v>
+      </c>
+      <c r="I193">
+        <v>0</v>
+      </c>
+      <c r="J193">
+        <v>1</v>
+      </c>
+      <c r="K193" t="s">
         <v>9</v>
       </c>
     </row>
@@ -50472,7 +52840,7 @@
   <dimension ref="A1:I210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
made changes to new csv file
</commit_message>
<xml_diff>
--- a/decision_data.xlsx
+++ b/decision_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/paul_kumar_mail_utoronto_ca/Documents/engineering_masters/thesis work/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D246D432-2AA5-4A25-8268-7CEE930D713B}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="6_{F6B86153-F216-4926-93F2-3946DCDAA96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BFE1708F-69BB-42DA-860D-63D46AB46265}"/>
   <bookViews>
-    <workbookView xWindow="-26115" yWindow="2685" windowWidth="21600" windowHeight="11385" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="3975" windowWidth="21600" windowHeight="11385" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="decision_data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="data_no_higher_order" sheetId="15" r:id="rId7"/>
     <sheet name="increased_gain" sheetId="16" r:id="rId8"/>
     <sheet name="schema_2" sheetId="17" r:id="rId9"/>
-    <sheet name="scheme_1" sheetId="19" r:id="rId10"/>
+    <sheet name="schema_1" sheetId="19" r:id="rId10"/>
     <sheet name="schema_2_continuous" sheetId="18" r:id="rId11"/>
   </sheets>
   <definedNames>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="29">
   <si>
     <t>first_peak</t>
   </si>
@@ -6567,14 +6567,26 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A1F1DB-53E2-4230-84C6-C3B0BD8E5FC9}">
-  <dimension ref="A1:K193"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2990638-EA7F-499C-9830-7D76C07FFC26}">
+  <dimension ref="A1:K125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K193"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -10948,2386 +10960,6 @@
         <v>1</v>
       </c>
       <c r="K125" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A126">
-        <v>1</v>
-      </c>
-      <c r="B126">
-        <v>0</v>
-      </c>
-      <c r="C126">
-        <v>0.12587834759376601</v>
-      </c>
-      <c r="D126">
-        <v>0</v>
-      </c>
-      <c r="E126">
-        <v>1</v>
-      </c>
-      <c r="F126">
-        <v>3.4911583468922001E-2</v>
-      </c>
-      <c r="G126">
-        <v>0</v>
-      </c>
-      <c r="H126">
-        <v>1</v>
-      </c>
-      <c r="I126">
-        <v>1</v>
-      </c>
-      <c r="J126">
-        <v>1</v>
-      </c>
-      <c r="K126" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A127">
-        <v>0</v>
-      </c>
-      <c r="B127">
-        <v>1</v>
-      </c>
-      <c r="C127">
-        <v>-6.9586179404461004E-2</v>
-      </c>
-      <c r="D127">
-        <v>1</v>
-      </c>
-      <c r="E127">
-        <v>1</v>
-      </c>
-      <c r="F127">
-        <v>3.1252497288195E-2</v>
-      </c>
-      <c r="G127">
-        <v>1</v>
-      </c>
-      <c r="H127">
-        <v>0</v>
-      </c>
-      <c r="I127">
-        <v>0</v>
-      </c>
-      <c r="J127">
-        <v>0</v>
-      </c>
-      <c r="K127" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A128">
-        <v>1</v>
-      </c>
-      <c r="B128">
-        <v>0</v>
-      </c>
-      <c r="C128">
-        <v>9.8359058045160999E-2</v>
-      </c>
-      <c r="D128">
-        <v>0</v>
-      </c>
-      <c r="E128">
-        <v>1</v>
-      </c>
-      <c r="F128">
-        <v>3.8313836869165001E-2</v>
-      </c>
-      <c r="G128">
-        <v>0</v>
-      </c>
-      <c r="H128">
-        <v>1</v>
-      </c>
-      <c r="I128">
-        <v>1</v>
-      </c>
-      <c r="J128">
-        <v>1</v>
-      </c>
-      <c r="K128" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129">
-        <v>1</v>
-      </c>
-      <c r="B129">
-        <v>0</v>
-      </c>
-      <c r="C129">
-        <v>0.135312389836899</v>
-      </c>
-      <c r="D129">
-        <v>1</v>
-      </c>
-      <c r="E129">
-        <v>1</v>
-      </c>
-      <c r="F129">
-        <v>0.12216818475437401</v>
-      </c>
-      <c r="G129">
-        <v>0</v>
-      </c>
-      <c r="H129">
-        <v>0</v>
-      </c>
-      <c r="I129">
-        <v>1</v>
-      </c>
-      <c r="J129">
-        <v>1</v>
-      </c>
-      <c r="K129" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A130">
-        <v>0</v>
-      </c>
-      <c r="B130">
-        <v>1</v>
-      </c>
-      <c r="C130">
-        <v>-2.9746967690679998E-2</v>
-      </c>
-      <c r="D130">
-        <v>0</v>
-      </c>
-      <c r="E130">
-        <v>0</v>
-      </c>
-      <c r="F130">
-        <v>4.7307840966217998E-2</v>
-      </c>
-      <c r="G130">
-        <v>1</v>
-      </c>
-      <c r="H130">
-        <v>1</v>
-      </c>
-      <c r="I130">
-        <v>0</v>
-      </c>
-      <c r="J130">
-        <v>1</v>
-      </c>
-      <c r="K130" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A131">
-        <v>1</v>
-      </c>
-      <c r="B131">
-        <v>0</v>
-      </c>
-      <c r="C131">
-        <v>6.7311247749722997E-2</v>
-      </c>
-      <c r="D131">
-        <v>1</v>
-      </c>
-      <c r="E131">
-        <v>1</v>
-      </c>
-      <c r="F131">
-        <v>3.1412841990926997E-2</v>
-      </c>
-      <c r="G131">
-        <v>0</v>
-      </c>
-      <c r="H131">
-        <v>0</v>
-      </c>
-      <c r="I131">
-        <v>1</v>
-      </c>
-      <c r="J131">
-        <v>1</v>
-      </c>
-      <c r="K131" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A132">
-        <v>0</v>
-      </c>
-      <c r="B132">
-        <v>1</v>
-      </c>
-      <c r="C132">
-        <v>-5.0151019876452999E-2</v>
-      </c>
-      <c r="D132">
-        <v>1</v>
-      </c>
-      <c r="E132">
-        <v>1</v>
-      </c>
-      <c r="F132">
-        <v>0.12721529553908301</v>
-      </c>
-      <c r="G132">
-        <v>1</v>
-      </c>
-      <c r="H132">
-        <v>0</v>
-      </c>
-      <c r="I132">
-        <v>0</v>
-      </c>
-      <c r="J132">
-        <v>1</v>
-      </c>
-      <c r="K132" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A133">
-        <v>1</v>
-      </c>
-      <c r="B133">
-        <v>0</v>
-      </c>
-      <c r="C133">
-        <v>3.8544184430813998E-2</v>
-      </c>
-      <c r="D133">
-        <v>1</v>
-      </c>
-      <c r="E133">
-        <v>1</v>
-      </c>
-      <c r="F133">
-        <v>-7.400012888535E-3</v>
-      </c>
-      <c r="G133">
-        <v>0</v>
-      </c>
-      <c r="H133">
-        <v>0</v>
-      </c>
-      <c r="I133">
-        <v>1</v>
-      </c>
-      <c r="J133">
-        <v>0</v>
-      </c>
-      <c r="K133" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A134">
-        <v>0</v>
-      </c>
-      <c r="B134">
-        <v>1</v>
-      </c>
-      <c r="C134">
-        <v>-1.8566986626454E-2</v>
-      </c>
-      <c r="D134">
-        <v>1</v>
-      </c>
-      <c r="E134">
-        <v>1</v>
-      </c>
-      <c r="F134">
-        <v>3.0652324702874999E-2</v>
-      </c>
-      <c r="G134">
-        <v>1</v>
-      </c>
-      <c r="H134">
-        <v>0</v>
-      </c>
-      <c r="I134">
-        <v>0</v>
-      </c>
-      <c r="J134">
-        <v>1</v>
-      </c>
-      <c r="K134" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A135">
-        <v>1</v>
-      </c>
-      <c r="B135">
-        <v>0</v>
-      </c>
-      <c r="C135">
-        <v>6.7482282286725995E-2</v>
-      </c>
-      <c r="D135">
-        <v>1</v>
-      </c>
-      <c r="E135">
-        <v>1</v>
-      </c>
-      <c r="F135">
-        <v>9.7814604588412998E-2</v>
-      </c>
-      <c r="G135">
-        <v>0</v>
-      </c>
-      <c r="H135">
-        <v>0</v>
-      </c>
-      <c r="I135">
-        <v>1</v>
-      </c>
-      <c r="J135">
-        <v>1</v>
-      </c>
-      <c r="K135" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A136">
-        <v>0</v>
-      </c>
-      <c r="B136">
-        <v>1</v>
-      </c>
-      <c r="C136">
-        <v>-7.0263159185719001E-2</v>
-      </c>
-      <c r="D136">
-        <v>1</v>
-      </c>
-      <c r="E136">
-        <v>1</v>
-      </c>
-      <c r="F136">
-        <v>0.18229620410880601</v>
-      </c>
-      <c r="G136">
-        <v>1</v>
-      </c>
-      <c r="H136">
-        <v>0</v>
-      </c>
-      <c r="I136">
-        <v>0</v>
-      </c>
-      <c r="J136">
-        <v>1</v>
-      </c>
-      <c r="K136" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A137">
-        <v>0</v>
-      </c>
-      <c r="B137">
-        <v>0</v>
-      </c>
-      <c r="C137">
-        <v>-1.7671020448010999E-2</v>
-      </c>
-      <c r="D137">
-        <v>1</v>
-      </c>
-      <c r="E137">
-        <v>1</v>
-      </c>
-      <c r="F137">
-        <v>0.114249096546259</v>
-      </c>
-      <c r="G137">
-        <v>1</v>
-      </c>
-      <c r="H137">
-        <v>0</v>
-      </c>
-      <c r="I137">
-        <v>1</v>
-      </c>
-      <c r="J137">
-        <v>1</v>
-      </c>
-      <c r="K137" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A138">
-        <v>1</v>
-      </c>
-      <c r="B138">
-        <v>1</v>
-      </c>
-      <c r="C138">
-        <v>-1.2199308180773E-2</v>
-      </c>
-      <c r="D138">
-        <v>1</v>
-      </c>
-      <c r="E138">
-        <v>1</v>
-      </c>
-      <c r="F138">
-        <v>0.24921467510915901</v>
-      </c>
-      <c r="G138">
-        <v>0</v>
-      </c>
-      <c r="H138">
-        <v>0</v>
-      </c>
-      <c r="I138">
-        <v>0</v>
-      </c>
-      <c r="J138">
-        <v>1</v>
-      </c>
-      <c r="K138" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A139">
-        <v>0</v>
-      </c>
-      <c r="B139">
-        <v>0</v>
-      </c>
-      <c r="C139">
-        <v>8.0092594456600003E-4</v>
-      </c>
-      <c r="D139">
-        <v>1</v>
-      </c>
-      <c r="E139">
-        <v>1</v>
-      </c>
-      <c r="F139">
-        <v>0.12930787271059699</v>
-      </c>
-      <c r="G139">
-        <v>1</v>
-      </c>
-      <c r="H139">
-        <v>0</v>
-      </c>
-      <c r="I139">
-        <v>1</v>
-      </c>
-      <c r="J139">
-        <v>1</v>
-      </c>
-      <c r="K139" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A140">
-        <v>1</v>
-      </c>
-      <c r="B140">
-        <v>0</v>
-      </c>
-      <c r="C140">
-        <v>0.13050344501354799</v>
-      </c>
-      <c r="D140">
-        <v>1</v>
-      </c>
-      <c r="E140">
-        <v>1</v>
-      </c>
-      <c r="F140">
-        <v>0</v>
-      </c>
-      <c r="G140">
-        <v>0</v>
-      </c>
-      <c r="H140">
-        <v>0</v>
-      </c>
-      <c r="I140">
-        <v>1</v>
-      </c>
-      <c r="J140">
-        <v>0</v>
-      </c>
-      <c r="K140" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A141">
-        <v>0</v>
-      </c>
-      <c r="B141">
-        <v>0</v>
-      </c>
-      <c r="C141">
-        <v>-0.121475329345405</v>
-      </c>
-      <c r="D141">
-        <v>1</v>
-      </c>
-      <c r="E141">
-        <v>1</v>
-      </c>
-      <c r="F141">
-        <v>7.5442564160345005E-2</v>
-      </c>
-      <c r="G141">
-        <v>1</v>
-      </c>
-      <c r="H141">
-        <v>0</v>
-      </c>
-      <c r="I141">
-        <v>1</v>
-      </c>
-      <c r="J141">
-        <v>0</v>
-      </c>
-      <c r="K141" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A142">
-        <v>1</v>
-      </c>
-      <c r="B142">
-        <v>0</v>
-      </c>
-      <c r="C142">
-        <v>5.4331416151837002E-2</v>
-      </c>
-      <c r="D142">
-        <v>1</v>
-      </c>
-      <c r="E142">
-        <v>0</v>
-      </c>
-      <c r="F142">
-        <v>8.8464491054556005E-2</v>
-      </c>
-      <c r="G142">
-        <v>0</v>
-      </c>
-      <c r="H142">
-        <v>0</v>
-      </c>
-      <c r="I142">
-        <v>1</v>
-      </c>
-      <c r="J142">
-        <v>1</v>
-      </c>
-      <c r="K142" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A143">
-        <v>1</v>
-      </c>
-      <c r="B143">
-        <v>1</v>
-      </c>
-      <c r="C143">
-        <v>2.4574020263507999E-2</v>
-      </c>
-      <c r="D143">
-        <v>0</v>
-      </c>
-      <c r="E143">
-        <v>0</v>
-      </c>
-      <c r="F143">
-        <v>2.8445782139730001E-2</v>
-      </c>
-      <c r="G143">
-        <v>0</v>
-      </c>
-      <c r="H143">
-        <v>1</v>
-      </c>
-      <c r="I143">
-        <v>0</v>
-      </c>
-      <c r="J143">
-        <v>1</v>
-      </c>
-      <c r="K143" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A144">
-        <v>1</v>
-      </c>
-      <c r="B144">
-        <v>0</v>
-      </c>
-      <c r="C144">
-        <v>6.7331902495410004E-2</v>
-      </c>
-      <c r="D144">
-        <v>0</v>
-      </c>
-      <c r="E144">
-        <v>1</v>
-      </c>
-      <c r="F144">
-        <v>2.3649724651075E-2</v>
-      </c>
-      <c r="G144">
-        <v>0</v>
-      </c>
-      <c r="H144">
-        <v>1</v>
-      </c>
-      <c r="I144">
-        <v>1</v>
-      </c>
-      <c r="J144">
-        <v>1</v>
-      </c>
-      <c r="K144" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A145">
-        <v>0</v>
-      </c>
-      <c r="B145">
-        <v>0</v>
-      </c>
-      <c r="C145">
-        <v>5.1507649474601E-2</v>
-      </c>
-      <c r="D145">
-        <v>1</v>
-      </c>
-      <c r="E145">
-        <v>0</v>
-      </c>
-      <c r="F145">
-        <v>0.122187262321728</v>
-      </c>
-      <c r="G145">
-        <v>1</v>
-      </c>
-      <c r="H145">
-        <v>0</v>
-      </c>
-      <c r="I145">
-        <v>1</v>
-      </c>
-      <c r="J145">
-        <v>1</v>
-      </c>
-      <c r="K145" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A146">
-        <v>1</v>
-      </c>
-      <c r="B146">
-        <v>0</v>
-      </c>
-      <c r="C146">
-        <v>0.12855152222590399</v>
-      </c>
-      <c r="D146">
-        <v>0</v>
-      </c>
-      <c r="E146">
-        <v>1</v>
-      </c>
-      <c r="F146">
-        <v>1.6747646704168E-2</v>
-      </c>
-      <c r="G146">
-        <v>0</v>
-      </c>
-      <c r="H146">
-        <v>1</v>
-      </c>
-      <c r="I146">
-        <v>1</v>
-      </c>
-      <c r="J146">
-        <v>0</v>
-      </c>
-      <c r="K146" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A147">
-        <v>0</v>
-      </c>
-      <c r="B147">
-        <v>1</v>
-      </c>
-      <c r="C147">
-        <v>-0.107968465455927</v>
-      </c>
-      <c r="D147">
-        <v>1</v>
-      </c>
-      <c r="E147">
-        <v>1</v>
-      </c>
-      <c r="F147">
-        <v>0.20004366522040601</v>
-      </c>
-      <c r="G147">
-        <v>1</v>
-      </c>
-      <c r="H147">
-        <v>0</v>
-      </c>
-      <c r="I147">
-        <v>0</v>
-      </c>
-      <c r="J147">
-        <v>0</v>
-      </c>
-      <c r="K147" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A148">
-        <v>1</v>
-      </c>
-      <c r="B148">
-        <v>0</v>
-      </c>
-      <c r="C148">
-        <v>0.11977190361734701</v>
-      </c>
-      <c r="D148">
-        <v>0</v>
-      </c>
-      <c r="E148">
-        <v>1</v>
-      </c>
-      <c r="F148">
-        <v>0.174196811839053</v>
-      </c>
-      <c r="G148">
-        <v>0</v>
-      </c>
-      <c r="H148">
-        <v>1</v>
-      </c>
-      <c r="I148">
-        <v>1</v>
-      </c>
-      <c r="J148">
-        <v>1</v>
-      </c>
-      <c r="K148" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A149">
-        <v>1</v>
-      </c>
-      <c r="B149">
-        <v>1</v>
-      </c>
-      <c r="C149">
-        <v>2.208570158259E-2</v>
-      </c>
-      <c r="D149">
-        <v>1</v>
-      </c>
-      <c r="E149">
-        <v>1</v>
-      </c>
-      <c r="F149">
-        <v>0.16656473244874301</v>
-      </c>
-      <c r="G149">
-        <v>0</v>
-      </c>
-      <c r="H149">
-        <v>0</v>
-      </c>
-      <c r="I149">
-        <v>0</v>
-      </c>
-      <c r="J149">
-        <v>0</v>
-      </c>
-      <c r="K149" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A150">
-        <v>1</v>
-      </c>
-      <c r="B150">
-        <v>0</v>
-      </c>
-      <c r="C150">
-        <v>0.11028810954889599</v>
-      </c>
-      <c r="D150">
-        <v>0</v>
-      </c>
-      <c r="E150">
-        <v>1</v>
-      </c>
-      <c r="F150">
-        <v>-7.2131916444890002E-3</v>
-      </c>
-      <c r="G150">
-        <v>0</v>
-      </c>
-      <c r="H150">
-        <v>1</v>
-      </c>
-      <c r="I150">
-        <v>1</v>
-      </c>
-      <c r="J150">
-        <v>0</v>
-      </c>
-      <c r="K150" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A151">
-        <v>1</v>
-      </c>
-      <c r="B151">
-        <v>0</v>
-      </c>
-      <c r="C151">
-        <v>0.164538788313775</v>
-      </c>
-      <c r="D151">
-        <v>1</v>
-      </c>
-      <c r="E151">
-        <v>1</v>
-      </c>
-      <c r="F151">
-        <v>0.19769080677557099</v>
-      </c>
-      <c r="G151">
-        <v>0</v>
-      </c>
-      <c r="H151">
-        <v>0</v>
-      </c>
-      <c r="I151">
-        <v>1</v>
-      </c>
-      <c r="J151">
-        <v>0</v>
-      </c>
-      <c r="K151" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A152">
-        <v>1</v>
-      </c>
-      <c r="B152">
-        <v>0</v>
-      </c>
-      <c r="C152">
-        <v>0.115841111204882</v>
-      </c>
-      <c r="D152">
-        <v>0</v>
-      </c>
-      <c r="E152">
-        <v>0</v>
-      </c>
-      <c r="F152">
-        <v>6.9944879180004998E-2</v>
-      </c>
-      <c r="G152">
-        <v>0</v>
-      </c>
-      <c r="H152">
-        <v>1</v>
-      </c>
-      <c r="I152">
-        <v>1</v>
-      </c>
-      <c r="J152">
-        <v>1</v>
-      </c>
-      <c r="K152" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A153">
-        <v>1</v>
-      </c>
-      <c r="B153">
-        <v>0</v>
-      </c>
-      <c r="C153">
-        <v>0.11222852490518501</v>
-      </c>
-      <c r="D153">
-        <v>1</v>
-      </c>
-      <c r="E153">
-        <v>0</v>
-      </c>
-      <c r="F153">
-        <v>0.258790586906259</v>
-      </c>
-      <c r="G153">
-        <v>0</v>
-      </c>
-      <c r="H153">
-        <v>0</v>
-      </c>
-      <c r="I153">
-        <v>1</v>
-      </c>
-      <c r="J153">
-        <v>1</v>
-      </c>
-      <c r="K153" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A154">
-        <v>1</v>
-      </c>
-      <c r="B154">
-        <v>0</v>
-      </c>
-      <c r="C154">
-        <v>0.107943409499644</v>
-      </c>
-      <c r="D154">
-        <v>0</v>
-      </c>
-      <c r="E154">
-        <v>0</v>
-      </c>
-      <c r="F154">
-        <v>0.147598323041503</v>
-      </c>
-      <c r="G154">
-        <v>0</v>
-      </c>
-      <c r="H154">
-        <v>1</v>
-      </c>
-      <c r="I154">
-        <v>1</v>
-      </c>
-      <c r="J154">
-        <v>1</v>
-      </c>
-      <c r="K154" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A155">
-        <v>1</v>
-      </c>
-      <c r="B155">
-        <v>1</v>
-      </c>
-      <c r="C155">
-        <v>-1.1428731271656001E-2</v>
-      </c>
-      <c r="D155">
-        <v>1</v>
-      </c>
-      <c r="E155">
-        <v>1</v>
-      </c>
-      <c r="F155">
-        <v>0.17832048849745899</v>
-      </c>
-      <c r="G155">
-        <v>0</v>
-      </c>
-      <c r="H155">
-        <v>0</v>
-      </c>
-      <c r="I155">
-        <v>0</v>
-      </c>
-      <c r="J155">
-        <v>0</v>
-      </c>
-      <c r="K155" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A156">
-        <v>1</v>
-      </c>
-      <c r="B156">
-        <v>0</v>
-      </c>
-      <c r="C156">
-        <v>0.12510275481264899</v>
-      </c>
-      <c r="D156">
-        <v>0</v>
-      </c>
-      <c r="E156">
-        <v>1</v>
-      </c>
-      <c r="F156">
-        <v>0.100298431429984</v>
-      </c>
-      <c r="G156">
-        <v>0</v>
-      </c>
-      <c r="H156">
-        <v>1</v>
-      </c>
-      <c r="I156">
-        <v>1</v>
-      </c>
-      <c r="J156">
-        <v>1</v>
-      </c>
-      <c r="K156" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A157">
-        <v>0</v>
-      </c>
-      <c r="B157">
-        <v>1</v>
-      </c>
-      <c r="C157">
-        <v>-0.122757792618454</v>
-      </c>
-      <c r="D157">
-        <v>1</v>
-      </c>
-      <c r="E157">
-        <v>1</v>
-      </c>
-      <c r="F157">
-        <v>0.278534734759467</v>
-      </c>
-      <c r="G157">
-        <v>1</v>
-      </c>
-      <c r="H157">
-        <v>0</v>
-      </c>
-      <c r="I157">
-        <v>0</v>
-      </c>
-      <c r="J157">
-        <v>0</v>
-      </c>
-      <c r="K157" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A158">
-        <v>1</v>
-      </c>
-      <c r="B158">
-        <v>0</v>
-      </c>
-      <c r="C158">
-        <v>6.0936821683702999E-2</v>
-      </c>
-      <c r="D158">
-        <v>0</v>
-      </c>
-      <c r="E158">
-        <v>0</v>
-      </c>
-      <c r="F158">
-        <v>3.5170315063290998E-2</v>
-      </c>
-      <c r="G158">
-        <v>0</v>
-      </c>
-      <c r="H158">
-        <v>1</v>
-      </c>
-      <c r="I158">
-        <v>1</v>
-      </c>
-      <c r="J158">
-        <v>1</v>
-      </c>
-      <c r="K158" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A159">
-        <v>0</v>
-      </c>
-      <c r="B159">
-        <v>0</v>
-      </c>
-      <c r="C159">
-        <v>-1.3278989861306E-2</v>
-      </c>
-      <c r="D159">
-        <v>1</v>
-      </c>
-      <c r="E159">
-        <v>1</v>
-      </c>
-      <c r="F159">
-        <v>0.24454415099542001</v>
-      </c>
-      <c r="G159">
-        <v>1</v>
-      </c>
-      <c r="H159">
-        <v>0</v>
-      </c>
-      <c r="I159">
-        <v>1</v>
-      </c>
-      <c r="J159">
-        <v>0</v>
-      </c>
-      <c r="K159" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A160">
-        <v>1</v>
-      </c>
-      <c r="B160">
-        <v>0</v>
-      </c>
-      <c r="C160">
-        <v>0.145737962503005</v>
-      </c>
-      <c r="D160">
-        <v>1</v>
-      </c>
-      <c r="E160">
-        <v>0</v>
-      </c>
-      <c r="F160">
-        <v>0.21381291530174201</v>
-      </c>
-      <c r="G160">
-        <v>0</v>
-      </c>
-      <c r="H160">
-        <v>0</v>
-      </c>
-      <c r="I160">
-        <v>1</v>
-      </c>
-      <c r="J160">
-        <v>1</v>
-      </c>
-      <c r="K160" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A161">
-        <v>1</v>
-      </c>
-      <c r="B161">
-        <v>0</v>
-      </c>
-      <c r="C161">
-        <v>-3.2360009542414997E-2</v>
-      </c>
-      <c r="D161">
-        <v>1</v>
-      </c>
-      <c r="E161">
-        <v>1</v>
-      </c>
-      <c r="F161">
-        <v>0.49155965593252399</v>
-      </c>
-      <c r="G161">
-        <v>0</v>
-      </c>
-      <c r="H161">
-        <v>0</v>
-      </c>
-      <c r="I161">
-        <v>1</v>
-      </c>
-      <c r="J161">
-        <v>1</v>
-      </c>
-      <c r="K161" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A162">
-        <v>1</v>
-      </c>
-      <c r="B162">
-        <v>0</v>
-      </c>
-      <c r="C162">
-        <v>0.10325941614380001</v>
-      </c>
-      <c r="D162">
-        <v>0</v>
-      </c>
-      <c r="E162">
-        <v>0</v>
-      </c>
-      <c r="F162">
-        <v>1.6386628311120002E-2</v>
-      </c>
-      <c r="G162">
-        <v>0</v>
-      </c>
-      <c r="H162">
-        <v>1</v>
-      </c>
-      <c r="I162">
-        <v>1</v>
-      </c>
-      <c r="J162">
-        <v>1</v>
-      </c>
-      <c r="K162" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A163">
-        <v>0</v>
-      </c>
-      <c r="B163">
-        <v>1</v>
-      </c>
-      <c r="C163">
-        <v>-0.14264009103695199</v>
-      </c>
-      <c r="D163">
-        <v>1</v>
-      </c>
-      <c r="E163">
-        <v>1</v>
-      </c>
-      <c r="F163">
-        <v>0.245771390082722</v>
-      </c>
-      <c r="G163">
-        <v>1</v>
-      </c>
-      <c r="H163">
-        <v>0</v>
-      </c>
-      <c r="I163">
-        <v>0</v>
-      </c>
-      <c r="J163">
-        <v>0</v>
-      </c>
-      <c r="K163" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A164">
-        <v>1</v>
-      </c>
-      <c r="B164">
-        <v>0</v>
-      </c>
-      <c r="C164">
-        <v>0.13021483995969399</v>
-      </c>
-      <c r="D164">
-        <v>1</v>
-      </c>
-      <c r="E164">
-        <v>1</v>
-      </c>
-      <c r="F164">
-        <v>0.15261205967334801</v>
-      </c>
-      <c r="G164">
-        <v>0</v>
-      </c>
-      <c r="H164">
-        <v>0</v>
-      </c>
-      <c r="I164">
-        <v>1</v>
-      </c>
-      <c r="J164">
-        <v>1</v>
-      </c>
-      <c r="K164" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A165">
-        <v>0</v>
-      </c>
-      <c r="B165">
-        <v>1</v>
-      </c>
-      <c r="C165">
-        <v>-0.18167735433553001</v>
-      </c>
-      <c r="D165">
-        <v>1</v>
-      </c>
-      <c r="E165">
-        <v>1</v>
-      </c>
-      <c r="F165">
-        <v>0.42678053946862499</v>
-      </c>
-      <c r="G165">
-        <v>1</v>
-      </c>
-      <c r="H165">
-        <v>0</v>
-      </c>
-      <c r="I165">
-        <v>0</v>
-      </c>
-      <c r="J165">
-        <v>1</v>
-      </c>
-      <c r="K165" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A166">
-        <v>1</v>
-      </c>
-      <c r="B166">
-        <v>0</v>
-      </c>
-      <c r="C166">
-        <v>0.115664688674583</v>
-      </c>
-      <c r="D166">
-        <v>1</v>
-      </c>
-      <c r="E166">
-        <v>0</v>
-      </c>
-      <c r="F166">
-        <v>0.16192762659069099</v>
-      </c>
-      <c r="G166">
-        <v>0</v>
-      </c>
-      <c r="H166">
-        <v>0</v>
-      </c>
-      <c r="I166">
-        <v>1</v>
-      </c>
-      <c r="J166">
-        <v>1</v>
-      </c>
-      <c r="K166" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A167">
-        <v>1</v>
-      </c>
-      <c r="B167">
-        <v>1</v>
-      </c>
-      <c r="C167">
-        <v>-6.5771644495389997E-3</v>
-      </c>
-      <c r="D167">
-        <v>1</v>
-      </c>
-      <c r="E167">
-        <v>1</v>
-      </c>
-      <c r="F167">
-        <v>0.27189608971817902</v>
-      </c>
-      <c r="G167">
-        <v>0</v>
-      </c>
-      <c r="H167">
-        <v>0</v>
-      </c>
-      <c r="I167">
-        <v>0</v>
-      </c>
-      <c r="J167">
-        <v>1</v>
-      </c>
-      <c r="K167" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A168">
-        <v>1</v>
-      </c>
-      <c r="B168">
-        <v>0</v>
-      </c>
-      <c r="C168">
-        <v>0.16346250043891999</v>
-      </c>
-      <c r="D168">
-        <v>1</v>
-      </c>
-      <c r="E168">
-        <v>1</v>
-      </c>
-      <c r="F168">
-        <v>0.16008220286330299</v>
-      </c>
-      <c r="G168">
-        <v>0</v>
-      </c>
-      <c r="H168">
-        <v>0</v>
-      </c>
-      <c r="I168">
-        <v>1</v>
-      </c>
-      <c r="J168">
-        <v>1</v>
-      </c>
-      <c r="K168" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A169">
-        <v>1</v>
-      </c>
-      <c r="B169">
-        <v>0</v>
-      </c>
-      <c r="C169">
-        <v>9.9075773954960006E-2</v>
-      </c>
-      <c r="D169">
-        <v>1</v>
-      </c>
-      <c r="E169">
-        <v>1</v>
-      </c>
-      <c r="F169">
-        <v>1.4963641870507E-2</v>
-      </c>
-      <c r="G169">
-        <v>0</v>
-      </c>
-      <c r="H169">
-        <v>0</v>
-      </c>
-      <c r="I169">
-        <v>1</v>
-      </c>
-      <c r="J169">
-        <v>0</v>
-      </c>
-      <c r="K169" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A170">
-        <v>0</v>
-      </c>
-      <c r="B170">
-        <v>1</v>
-      </c>
-      <c r="C170">
-        <v>-4.9000556221567002E-2</v>
-      </c>
-      <c r="D170">
-        <v>1</v>
-      </c>
-      <c r="E170">
-        <v>1</v>
-      </c>
-      <c r="F170">
-        <v>6.2209633171937999E-2</v>
-      </c>
-      <c r="G170">
-        <v>1</v>
-      </c>
-      <c r="H170">
-        <v>0</v>
-      </c>
-      <c r="I170">
-        <v>0</v>
-      </c>
-      <c r="J170">
-        <v>0</v>
-      </c>
-      <c r="K170" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A171">
-        <v>1</v>
-      </c>
-      <c r="B171">
-        <v>0</v>
-      </c>
-      <c r="C171">
-        <v>0.102057254290186</v>
-      </c>
-      <c r="D171">
-        <v>0</v>
-      </c>
-      <c r="E171">
-        <v>1</v>
-      </c>
-      <c r="F171">
-        <v>2.0021098484447001E-2</v>
-      </c>
-      <c r="G171">
-        <v>0</v>
-      </c>
-      <c r="H171">
-        <v>1</v>
-      </c>
-      <c r="I171">
-        <v>1</v>
-      </c>
-      <c r="J171">
-        <v>1</v>
-      </c>
-      <c r="K171" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A172">
-        <v>0</v>
-      </c>
-      <c r="B172">
-        <v>1</v>
-      </c>
-      <c r="C172">
-        <v>-7.1380801464027005E-2</v>
-      </c>
-      <c r="D172">
-        <v>1</v>
-      </c>
-      <c r="E172">
-        <v>1</v>
-      </c>
-      <c r="F172">
-        <v>3.2219859614870998E-2</v>
-      </c>
-      <c r="G172">
-        <v>1</v>
-      </c>
-      <c r="H172">
-        <v>0</v>
-      </c>
-      <c r="I172">
-        <v>0</v>
-      </c>
-      <c r="J172">
-        <v>0</v>
-      </c>
-      <c r="K172" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A173">
-        <v>1</v>
-      </c>
-      <c r="B173">
-        <v>0</v>
-      </c>
-      <c r="C173">
-        <v>5.3751833559836003E-2</v>
-      </c>
-      <c r="D173">
-        <v>1</v>
-      </c>
-      <c r="E173">
-        <v>1</v>
-      </c>
-      <c r="F173">
-        <v>-1.6025162267238002E-2</v>
-      </c>
-      <c r="G173">
-        <v>0</v>
-      </c>
-      <c r="H173">
-        <v>0</v>
-      </c>
-      <c r="I173">
-        <v>1</v>
-      </c>
-      <c r="J173">
-        <v>0</v>
-      </c>
-      <c r="K173" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A174">
-        <v>0</v>
-      </c>
-      <c r="B174">
-        <v>1</v>
-      </c>
-      <c r="C174">
-        <v>-6.2642348962186997E-2</v>
-      </c>
-      <c r="D174">
-        <v>1</v>
-      </c>
-      <c r="E174">
-        <v>0</v>
-      </c>
-      <c r="F174">
-        <v>8.5448174226623E-2</v>
-      </c>
-      <c r="G174">
-        <v>1</v>
-      </c>
-      <c r="H174">
-        <v>0</v>
-      </c>
-      <c r="I174">
-        <v>0</v>
-      </c>
-      <c r="J174">
-        <v>1</v>
-      </c>
-      <c r="K174" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A175">
-        <v>1</v>
-      </c>
-      <c r="B175">
-        <v>0</v>
-      </c>
-      <c r="C175">
-        <v>8.5067604183791001E-2</v>
-      </c>
-      <c r="D175">
-        <v>0</v>
-      </c>
-      <c r="E175">
-        <v>1</v>
-      </c>
-      <c r="F175">
-        <v>-2.6146569607001E-2</v>
-      </c>
-      <c r="G175">
-        <v>0</v>
-      </c>
-      <c r="H175">
-        <v>1</v>
-      </c>
-      <c r="I175">
-        <v>1</v>
-      </c>
-      <c r="J175">
-        <v>0</v>
-      </c>
-      <c r="K175" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A176">
-        <v>0</v>
-      </c>
-      <c r="B176">
-        <v>1</v>
-      </c>
-      <c r="C176">
-        <v>-4.1026934093399997E-2</v>
-      </c>
-      <c r="D176">
-        <v>1</v>
-      </c>
-      <c r="E176">
-        <v>1</v>
-      </c>
-      <c r="F176">
-        <v>0.257558816919154</v>
-      </c>
-      <c r="G176">
-        <v>1</v>
-      </c>
-      <c r="H176">
-        <v>0</v>
-      </c>
-      <c r="I176">
-        <v>0</v>
-      </c>
-      <c r="J176">
-        <v>1</v>
-      </c>
-      <c r="K176" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A177">
-        <v>1</v>
-      </c>
-      <c r="B177">
-        <v>0</v>
-      </c>
-      <c r="C177">
-        <v>3.7423699240194001E-2</v>
-      </c>
-      <c r="D177">
-        <v>1</v>
-      </c>
-      <c r="E177">
-        <v>1</v>
-      </c>
-      <c r="F177">
-        <v>5.7804717541829996E-3</v>
-      </c>
-      <c r="G177">
-        <v>0</v>
-      </c>
-      <c r="H177">
-        <v>0</v>
-      </c>
-      <c r="I177">
-        <v>1</v>
-      </c>
-      <c r="J177">
-        <v>0</v>
-      </c>
-      <c r="K177" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A178">
-        <v>0</v>
-      </c>
-      <c r="B178">
-        <v>1</v>
-      </c>
-      <c r="C178">
-        <v>-6.1874523818413997E-2</v>
-      </c>
-      <c r="D178">
-        <v>0</v>
-      </c>
-      <c r="E178">
-        <v>1</v>
-      </c>
-      <c r="F178">
-        <v>-1.727017648673E-3</v>
-      </c>
-      <c r="G178">
-        <v>1</v>
-      </c>
-      <c r="H178">
-        <v>1</v>
-      </c>
-      <c r="I178">
-        <v>0</v>
-      </c>
-      <c r="J178">
-        <v>0</v>
-      </c>
-      <c r="K178" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A179">
-        <v>1</v>
-      </c>
-      <c r="B179">
-        <v>1</v>
-      </c>
-      <c r="C179">
-        <v>0.121334620593191</v>
-      </c>
-      <c r="D179">
-        <v>1</v>
-      </c>
-      <c r="E179">
-        <v>1</v>
-      </c>
-      <c r="F179">
-        <v>-1.8433882879413999E-2</v>
-      </c>
-      <c r="G179">
-        <v>0</v>
-      </c>
-      <c r="H179">
-        <v>0</v>
-      </c>
-      <c r="I179">
-        <v>0</v>
-      </c>
-      <c r="J179">
-        <v>0</v>
-      </c>
-      <c r="K179" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A180">
-        <v>1</v>
-      </c>
-      <c r="B180">
-        <v>0</v>
-      </c>
-      <c r="C180">
-        <v>9.6680478559113006E-2</v>
-      </c>
-      <c r="D180">
-        <v>0</v>
-      </c>
-      <c r="E180">
-        <v>1</v>
-      </c>
-      <c r="F180">
-        <v>8.3571593391845E-2</v>
-      </c>
-      <c r="G180">
-        <v>0</v>
-      </c>
-      <c r="H180">
-        <v>1</v>
-      </c>
-      <c r="I180">
-        <v>1</v>
-      </c>
-      <c r="J180">
-        <v>1</v>
-      </c>
-      <c r="K180" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A181">
-        <v>1</v>
-      </c>
-      <c r="B181">
-        <v>0</v>
-      </c>
-      <c r="C181">
-        <v>8.3485766432251002E-2</v>
-      </c>
-      <c r="D181">
-        <v>1</v>
-      </c>
-      <c r="E181">
-        <v>1</v>
-      </c>
-      <c r="F181">
-        <v>-2.4235489941359998E-3</v>
-      </c>
-      <c r="G181">
-        <v>0</v>
-      </c>
-      <c r="H181">
-        <v>0</v>
-      </c>
-      <c r="I181">
-        <v>1</v>
-      </c>
-      <c r="J181">
-        <v>0</v>
-      </c>
-      <c r="K181" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A182">
-        <v>0</v>
-      </c>
-      <c r="B182">
-        <v>0</v>
-      </c>
-      <c r="C182">
-        <v>-3.5033668162458002E-2</v>
-      </c>
-      <c r="D182">
-        <v>1</v>
-      </c>
-      <c r="E182">
-        <v>0</v>
-      </c>
-      <c r="F182">
-        <v>9.0226586238517995E-2</v>
-      </c>
-      <c r="G182">
-        <v>1</v>
-      </c>
-      <c r="H182">
-        <v>0</v>
-      </c>
-      <c r="I182">
-        <v>1</v>
-      </c>
-      <c r="J182">
-        <v>1</v>
-      </c>
-      <c r="K182" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A183">
-        <v>1</v>
-      </c>
-      <c r="B183">
-        <v>0</v>
-      </c>
-      <c r="C183">
-        <v>9.8813416764808995E-2</v>
-      </c>
-      <c r="D183">
-        <v>1</v>
-      </c>
-      <c r="E183">
-        <v>0</v>
-      </c>
-      <c r="F183">
-        <v>7.2200216511165996E-2</v>
-      </c>
-      <c r="G183">
-        <v>0</v>
-      </c>
-      <c r="H183">
-        <v>0</v>
-      </c>
-      <c r="I183">
-        <v>1</v>
-      </c>
-      <c r="J183">
-        <v>1</v>
-      </c>
-      <c r="K183" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A184">
-        <v>0</v>
-      </c>
-      <c r="B184">
-        <v>0</v>
-      </c>
-      <c r="C184">
-        <v>3.6429096606767998E-2</v>
-      </c>
-      <c r="D184">
-        <v>1</v>
-      </c>
-      <c r="E184">
-        <v>1</v>
-      </c>
-      <c r="F184">
-        <v>2.2699645821509999E-3</v>
-      </c>
-      <c r="G184">
-        <v>1</v>
-      </c>
-      <c r="H184">
-        <v>0</v>
-      </c>
-      <c r="I184">
-        <v>1</v>
-      </c>
-      <c r="J184">
-        <v>0</v>
-      </c>
-      <c r="K184" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A185">
-        <v>1</v>
-      </c>
-      <c r="B185">
-        <v>1</v>
-      </c>
-      <c r="C185">
-        <v>7.0115361094648998E-2</v>
-      </c>
-      <c r="D185">
-        <v>1</v>
-      </c>
-      <c r="E185">
-        <v>1</v>
-      </c>
-      <c r="F185">
-        <v>4.4310171888179997E-2</v>
-      </c>
-      <c r="G185">
-        <v>0</v>
-      </c>
-      <c r="H185">
-        <v>0</v>
-      </c>
-      <c r="I185">
-        <v>0</v>
-      </c>
-      <c r="J185">
-        <v>0</v>
-      </c>
-      <c r="K185" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A186">
-        <v>1</v>
-      </c>
-      <c r="B186">
-        <v>0</v>
-      </c>
-      <c r="C186">
-        <v>4.3129725917827003E-2</v>
-      </c>
-      <c r="D186">
-        <v>1</v>
-      </c>
-      <c r="E186">
-        <v>1</v>
-      </c>
-      <c r="F186">
-        <v>5.7085456422907001E-2</v>
-      </c>
-      <c r="G186">
-        <v>0</v>
-      </c>
-      <c r="H186">
-        <v>0</v>
-      </c>
-      <c r="I186">
-        <v>1</v>
-      </c>
-      <c r="J186">
-        <v>1</v>
-      </c>
-      <c r="K186" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A187">
-        <v>0</v>
-      </c>
-      <c r="B187">
-        <v>1</v>
-      </c>
-      <c r="C187">
-        <v>-3.3297925541104001E-2</v>
-      </c>
-      <c r="D187">
-        <v>1</v>
-      </c>
-      <c r="E187">
-        <v>1</v>
-      </c>
-      <c r="F187">
-        <v>7.8133431767489995E-3</v>
-      </c>
-      <c r="G187">
-        <v>1</v>
-      </c>
-      <c r="H187">
-        <v>0</v>
-      </c>
-      <c r="I187">
-        <v>0</v>
-      </c>
-      <c r="J187">
-        <v>0</v>
-      </c>
-      <c r="K187" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A188">
-        <v>1</v>
-      </c>
-      <c r="B188">
-        <v>0</v>
-      </c>
-      <c r="C188">
-        <v>0.106358299154435</v>
-      </c>
-      <c r="D188">
-        <v>0</v>
-      </c>
-      <c r="E188">
-        <v>1</v>
-      </c>
-      <c r="F188">
-        <v>-5.3710240442535001E-2</v>
-      </c>
-      <c r="G188">
-        <v>0</v>
-      </c>
-      <c r="H188">
-        <v>1</v>
-      </c>
-      <c r="I188">
-        <v>1</v>
-      </c>
-      <c r="J188">
-        <v>0</v>
-      </c>
-      <c r="K188" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A189">
-        <v>0</v>
-      </c>
-      <c r="B189">
-        <v>0</v>
-      </c>
-      <c r="C189">
-        <v>-3.1682587699729002E-2</v>
-      </c>
-      <c r="D189">
-        <v>1</v>
-      </c>
-      <c r="E189">
-        <v>1</v>
-      </c>
-      <c r="F189">
-        <v>6.7197061656886006E-2</v>
-      </c>
-      <c r="G189">
-        <v>1</v>
-      </c>
-      <c r="H189">
-        <v>0</v>
-      </c>
-      <c r="I189">
-        <v>1</v>
-      </c>
-      <c r="J189">
-        <v>0</v>
-      </c>
-      <c r="K189" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A190">
-        <v>1</v>
-      </c>
-      <c r="B190">
-        <v>0</v>
-      </c>
-      <c r="C190">
-        <v>7.2168419648430002E-2</v>
-      </c>
-      <c r="D190">
-        <v>1</v>
-      </c>
-      <c r="E190">
-        <v>0</v>
-      </c>
-      <c r="F190">
-        <v>6.7835195800275999E-2</v>
-      </c>
-      <c r="G190">
-        <v>0</v>
-      </c>
-      <c r="H190">
-        <v>0</v>
-      </c>
-      <c r="I190">
-        <v>1</v>
-      </c>
-      <c r="J190">
-        <v>1</v>
-      </c>
-      <c r="K190" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A191">
-        <v>1</v>
-      </c>
-      <c r="B191">
-        <v>1</v>
-      </c>
-      <c r="C191">
-        <v>-2.023650852169E-3</v>
-      </c>
-      <c r="D191">
-        <v>1</v>
-      </c>
-      <c r="E191">
-        <v>1</v>
-      </c>
-      <c r="F191">
-        <v>0.17615785772753201</v>
-      </c>
-      <c r="G191">
-        <v>0</v>
-      </c>
-      <c r="H191">
-        <v>0</v>
-      </c>
-      <c r="I191">
-        <v>0</v>
-      </c>
-      <c r="J191">
-        <v>1</v>
-      </c>
-      <c r="K191" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A192">
-        <v>1</v>
-      </c>
-      <c r="B192">
-        <v>0</v>
-      </c>
-      <c r="C192">
-        <v>-5.7332836462008999E-2</v>
-      </c>
-      <c r="D192">
-        <v>0</v>
-      </c>
-      <c r="E192">
-        <v>0</v>
-      </c>
-      <c r="F192">
-        <v>0.31792420655674303</v>
-      </c>
-      <c r="G192">
-        <v>0</v>
-      </c>
-      <c r="H192">
-        <v>1</v>
-      </c>
-      <c r="I192">
-        <v>1</v>
-      </c>
-      <c r="J192">
-        <v>1</v>
-      </c>
-      <c r="K192" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A193">
-        <v>1</v>
-      </c>
-      <c r="B193">
-        <v>1</v>
-      </c>
-      <c r="C193">
-        <v>4.9444954157733E-2</v>
-      </c>
-      <c r="D193">
-        <v>1</v>
-      </c>
-      <c r="E193">
-        <v>0</v>
-      </c>
-      <c r="F193">
-        <v>8.6611415019430996E-2</v>
-      </c>
-      <c r="G193">
-        <v>0</v>
-      </c>
-      <c r="H193">
-        <v>0</v>
-      </c>
-      <c r="I193">
-        <v>0</v>
-      </c>
-      <c r="J193">
-        <v>1</v>
-      </c>
-      <c r="K193" t="s">
         <v>9</v>
       </c>
     </row>
@@ -52840,7 +50472,7 @@
   <dimension ref="A1:I210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>